<commit_message>
Sorted SSAO memory measurements
</commit_message>
<xml_diff>
--- a/Experiment/Results/MemoryUsageSorted.xlsx
+++ b/Experiment/Results/MemoryUsageSorted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Howest\GD_J3_S2\Gradwork_2.0\Gradwork\Experiment\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D49EB18-9BB1-4BD8-9A11-B13D3F253A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F615D0E2-6CA5-4C60-BF6D-C2E36107C3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22550" yWindow="-10100" windowWidth="16430" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-10790" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SSAO" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +104,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -307,13 +325,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1"/>
@@ -333,11 +354,23 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="7">
+    <cellStyle name="20% - Accent2" xfId="4" builtinId="34"/>
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
+    <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
     <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent2" xfId="6" builtinId="36"/>
     <cellStyle name="60% - Accent6" xfId="3" builtinId="52"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -619,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,19 +679,19 @@
       <c r="D3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="24">
         <v>1</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="24">
         <v>2</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="24">
         <v>3</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="24">
         <v>4</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="24">
         <v>5</v>
       </c>
       <c r="J3" s="17">
@@ -691,19 +724,19 @@
       <c r="S3" s="17">
         <v>15</v>
       </c>
-      <c r="T3" s="17">
+      <c r="T3" s="24">
         <v>16</v>
       </c>
-      <c r="U3" s="17">
+      <c r="U3" s="24">
         <v>17</v>
       </c>
-      <c r="V3" s="17">
+      <c r="V3" s="24">
         <v>18</v>
       </c>
-      <c r="W3" s="16">
+      <c r="W3" s="25">
         <v>19</v>
       </c>
-      <c r="X3" s="17">
+      <c r="X3" s="24">
         <v>20</v>
       </c>
     </row>
@@ -715,41 +748,41 @@
         <v>1</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D4:D15" si="0">AVERAGE(E4:AC4)</f>
-        <v>514.79999999999995</v>
-      </c>
-      <c r="E4" s="3">
+        <f>AVERAGE(J4:S4)</f>
+        <v>514.9</v>
+      </c>
+      <c r="E4" s="19">
+        <v>511</v>
+      </c>
+      <c r="F4" s="19">
         <v>512</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="19">
+        <v>512</v>
+      </c>
+      <c r="H4" s="19">
+        <v>512</v>
+      </c>
+      <c r="I4" s="19">
         <v>513</v>
       </c>
-      <c r="G4" s="3">
-        <v>516</v>
-      </c>
-      <c r="H4" s="3">
-        <v>517</v>
-      </c>
-      <c r="I4" s="3">
-        <v>516</v>
-      </c>
       <c r="J4" s="3">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K4" s="3">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="L4" s="3">
         <v>513</v>
       </c>
       <c r="M4" s="3">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="N4" s="3">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="O4" s="3">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="P4" s="3">
         <v>516</v>
@@ -761,22 +794,22 @@
         <v>516</v>
       </c>
       <c r="S4" s="3">
-        <v>512</v>
-      </c>
-      <c r="T4" s="3">
-        <v>512</v>
-      </c>
-      <c r="U4" s="3">
+        <v>516</v>
+      </c>
+      <c r="T4" s="19">
+        <v>517</v>
+      </c>
+      <c r="U4" s="19">
+        <v>517</v>
+      </c>
+      <c r="V4" s="21">
+        <v>517</v>
+      </c>
+      <c r="W4" s="22">
         <v>518</v>
       </c>
-      <c r="V4" s="19">
-        <v>513</v>
-      </c>
-      <c r="W4" s="2">
-        <v>517</v>
-      </c>
-      <c r="X4" s="3">
-        <v>515</v>
+      <c r="X4" s="19">
+        <v>518</v>
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.3">
@@ -787,68 +820,68 @@
         <v>2</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="0"/>
-        <v>689.6</v>
-      </c>
-      <c r="E5" s="6">
+        <f t="shared" ref="D5:D15" si="0">AVERAGE(J5:S5)</f>
+        <v>687.1</v>
+      </c>
+      <c r="E5" s="20">
         <v>684</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="20">
+        <v>684</v>
+      </c>
+      <c r="G5" s="20">
+        <v>685</v>
+      </c>
+      <c r="H5" s="20">
+        <v>685</v>
+      </c>
+      <c r="I5" s="20">
         <v>686</v>
       </c>
-      <c r="G5" s="6">
+      <c r="J5" s="6">
         <v>686</v>
       </c>
-      <c r="H5" s="6">
+      <c r="K5" s="6">
         <v>686</v>
       </c>
-      <c r="I5" s="6">
+      <c r="L5" s="6">
         <v>686</v>
       </c>
-      <c r="J5" s="6">
+      <c r="M5" s="6">
+        <v>686</v>
+      </c>
+      <c r="N5" s="6">
         <v>687</v>
       </c>
-      <c r="K5" s="6">
-        <v>693</v>
-      </c>
-      <c r="L5" s="6">
-        <v>685</v>
-      </c>
-      <c r="M5" s="6">
-        <v>703</v>
-      </c>
-      <c r="N5" s="6">
-        <v>708</v>
-      </c>
       <c r="O5" s="6">
-        <v>703</v>
+        <v>687</v>
       </c>
       <c r="P5" s="6">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="Q5" s="6">
         <v>688</v>
       </c>
       <c r="R5" s="6">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="S5" s="6">
         <v>690</v>
       </c>
-      <c r="T5" s="6">
-        <v>685</v>
-      </c>
-      <c r="U5" s="6">
-        <v>688</v>
-      </c>
-      <c r="V5" s="6">
-        <v>686</v>
-      </c>
-      <c r="W5" s="5">
-        <v>687</v>
-      </c>
-      <c r="X5" s="6">
+      <c r="T5" s="20">
         <v>690</v>
+      </c>
+      <c r="U5" s="20">
+        <v>693</v>
+      </c>
+      <c r="V5" s="20">
+        <v>703</v>
+      </c>
+      <c r="W5" s="23">
+        <v>703</v>
+      </c>
+      <c r="X5" s="20">
+        <v>708</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
@@ -860,67 +893,67 @@
       </c>
       <c r="D6" s="3">
         <f t="shared" si="0"/>
-        <v>1293.45</v>
-      </c>
-      <c r="E6" s="6">
+        <v>1290</v>
+      </c>
+      <c r="E6" s="20">
+        <v>1287</v>
+      </c>
+      <c r="F6" s="20">
+        <v>1287</v>
+      </c>
+      <c r="G6" s="20">
         <v>1288</v>
       </c>
-      <c r="F6" s="6">
+      <c r="H6" s="20">
         <v>1288</v>
       </c>
-      <c r="G6" s="6">
-        <v>1287</v>
-      </c>
-      <c r="H6" s="6">
+      <c r="I6" s="20">
+        <v>1288</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1288</v>
+      </c>
+      <c r="K6" s="6">
         <v>1289</v>
       </c>
-      <c r="I6" s="6">
+      <c r="L6" s="6">
+        <v>1289</v>
+      </c>
+      <c r="M6" s="6">
+        <v>1289</v>
+      </c>
+      <c r="N6" s="6">
+        <v>1289</v>
+      </c>
+      <c r="O6" s="6">
+        <v>1290</v>
+      </c>
+      <c r="P6" s="6">
+        <v>1290</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>1291</v>
+      </c>
+      <c r="R6" s="6">
+        <v>1292</v>
+      </c>
+      <c r="S6" s="6">
+        <v>1293</v>
+      </c>
+      <c r="T6" s="20">
+        <v>1304</v>
+      </c>
+      <c r="U6" s="20">
         <v>1305</v>
       </c>
-      <c r="J6" s="6">
-        <v>1289</v>
-      </c>
-      <c r="K6" s="6">
-        <v>1292</v>
-      </c>
-      <c r="L6" s="6">
-        <v>1291</v>
-      </c>
-      <c r="M6" s="6">
-        <v>1304</v>
-      </c>
-      <c r="N6" s="6">
+      <c r="V6" s="20">
+        <v>1306</v>
+      </c>
+      <c r="W6" s="23">
         <v>1307</v>
       </c>
-      <c r="O6" s="6">
-        <v>1306</v>
-      </c>
-      <c r="P6" s="6">
-        <v>1289</v>
-      </c>
-      <c r="Q6" s="6">
-        <v>1293</v>
-      </c>
-      <c r="R6" s="6">
-        <v>1289</v>
-      </c>
-      <c r="S6" s="6">
-        <v>1290</v>
-      </c>
-      <c r="T6" s="6">
-        <v>1287</v>
-      </c>
-      <c r="U6" s="6">
-        <v>1290</v>
-      </c>
-      <c r="V6" s="6">
-        <v>1288</v>
-      </c>
-      <c r="W6" s="5">
+      <c r="X6" s="20">
         <v>1309</v>
-      </c>
-      <c r="X6" s="6">
-        <v>1288</v>
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
@@ -930,69 +963,69 @@
       <c r="C7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>517.35</v>
-      </c>
-      <c r="E7" s="10">
-        <v>515</v>
-      </c>
-      <c r="F7" s="10">
+        <v>514.70000000000005</v>
+      </c>
+      <c r="E7" s="27">
         <v>511</v>
       </c>
-      <c r="G7" s="10">
+      <c r="F7" s="27">
+        <v>512</v>
+      </c>
+      <c r="G7" s="27">
         <v>513</v>
       </c>
-      <c r="H7" s="10">
-        <v>533</v>
-      </c>
-      <c r="I7" s="10">
-        <v>515</v>
+      <c r="H7" s="27">
+        <v>513</v>
+      </c>
+      <c r="I7" s="27">
+        <v>514</v>
       </c>
       <c r="J7" s="10">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="K7" s="10">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="L7" s="10">
         <v>514</v>
       </c>
       <c r="M7" s="10">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="N7" s="10">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="O7" s="10">
-        <v>539</v>
+        <v>515</v>
       </c>
       <c r="P7" s="10">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="Q7" s="10">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="R7" s="10">
         <v>515</v>
       </c>
       <c r="S7" s="10">
-        <v>514</v>
-      </c>
-      <c r="T7" s="10">
+        <v>516</v>
+      </c>
+      <c r="T7" s="27">
+        <v>516</v>
+      </c>
+      <c r="U7" s="27">
+        <v>517</v>
+      </c>
+      <c r="V7" s="27">
         <v>532</v>
       </c>
-      <c r="U7" s="10">
-        <v>515</v>
-      </c>
-      <c r="V7" s="10">
-        <v>516</v>
-      </c>
-      <c r="W7" s="8">
-        <v>513</v>
-      </c>
-      <c r="X7" s="10">
-        <v>514</v>
+      <c r="W7" s="28">
+        <v>533</v>
+      </c>
+      <c r="X7" s="27">
+        <v>539</v>
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
@@ -1002,69 +1035,69 @@
       <c r="C8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>699.05</v>
-      </c>
-      <c r="E8" s="10">
-        <v>706</v>
-      </c>
-      <c r="F8" s="10">
+        <v>702.1</v>
+      </c>
+      <c r="E8" s="27">
+        <v>683</v>
+      </c>
+      <c r="F8" s="27">
+        <v>684</v>
+      </c>
+      <c r="G8" s="27">
+        <v>686</v>
+      </c>
+      <c r="H8" s="27">
+        <v>686</v>
+      </c>
+      <c r="I8" s="27">
+        <v>686</v>
+      </c>
+      <c r="J8" s="10">
+        <v>687</v>
+      </c>
+      <c r="K8" s="10">
+        <v>701</v>
+      </c>
+      <c r="L8" s="10">
+        <v>702</v>
+      </c>
+      <c r="M8" s="10">
+        <v>703</v>
+      </c>
+      <c r="N8" s="10">
         <v>704</v>
       </c>
-      <c r="G8" s="10">
-        <v>683</v>
-      </c>
-      <c r="H8" s="10">
-        <v>701</v>
-      </c>
-      <c r="I8" s="10">
+      <c r="O8" s="10">
         <v>704</v>
       </c>
-      <c r="J8" s="10">
-        <v>703</v>
-      </c>
-      <c r="K8" s="10">
+      <c r="P8" s="10">
         <v>704</v>
-      </c>
-      <c r="L8" s="10">
-        <v>710</v>
-      </c>
-      <c r="M8" s="10">
-        <v>686</v>
-      </c>
-      <c r="N8" s="10">
-        <v>706</v>
-      </c>
-      <c r="O8" s="10">
-        <v>707</v>
-      </c>
-      <c r="P8" s="10">
-        <v>706</v>
       </c>
       <c r="Q8" s="10">
         <v>705</v>
       </c>
       <c r="R8" s="10">
-        <v>686</v>
+        <v>705</v>
       </c>
       <c r="S8" s="10">
-        <v>687</v>
-      </c>
-      <c r="T8" s="10">
-        <v>702</v>
-      </c>
-      <c r="U8" s="10">
         <v>706</v>
       </c>
-      <c r="V8" s="10">
-        <v>705</v>
-      </c>
-      <c r="W8" s="8">
-        <v>684</v>
-      </c>
-      <c r="X8" s="10">
-        <v>686</v>
+      <c r="T8" s="27">
+        <v>706</v>
+      </c>
+      <c r="U8" s="27">
+        <v>706</v>
+      </c>
+      <c r="V8" s="27">
+        <v>706</v>
+      </c>
+      <c r="W8" s="28">
+        <v>707</v>
+      </c>
+      <c r="X8" s="27">
+        <v>710</v>
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
@@ -1074,69 +1107,69 @@
       <c r="C9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
-        <v>1303.1500000000001</v>
-      </c>
-      <c r="E9" s="10">
-        <v>1307</v>
-      </c>
-      <c r="F9" s="10">
+        <v>1306.0999999999999</v>
+      </c>
+      <c r="E9" s="27">
+        <v>1287</v>
+      </c>
+      <c r="F9" s="27">
+        <v>1288</v>
+      </c>
+      <c r="G9" s="27">
+        <v>1289</v>
+      </c>
+      <c r="H9" s="27">
+        <v>1291</v>
+      </c>
+      <c r="I9" s="27">
         <v>1305</v>
       </c>
-      <c r="G9" s="10">
+      <c r="J9" s="10">
         <v>1305</v>
       </c>
-      <c r="H9" s="10">
-        <v>1308</v>
-      </c>
-      <c r="I9" s="10">
+      <c r="K9" s="10">
         <v>1305</v>
-      </c>
-      <c r="J9" s="10">
-        <v>1309</v>
-      </c>
-      <c r="K9" s="10">
-        <v>1307</v>
       </c>
       <c r="L9" s="10">
         <v>1306</v>
       </c>
       <c r="M9" s="10">
-        <v>1291</v>
+        <v>1306</v>
       </c>
       <c r="N9" s="10">
-        <v>1309</v>
+        <v>1306</v>
       </c>
       <c r="O9" s="10">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="P9" s="10">
         <v>1306</v>
       </c>
       <c r="Q9" s="10">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="R9" s="10">
-        <v>1288</v>
+        <v>1307</v>
       </c>
       <c r="S9" s="10">
         <v>1307</v>
       </c>
-      <c r="T9" s="10">
-        <v>1306</v>
-      </c>
-      <c r="U9" s="10">
-        <v>1306</v>
-      </c>
-      <c r="V9" s="10">
-        <v>1306</v>
-      </c>
-      <c r="W9" s="8">
-        <v>1289</v>
-      </c>
-      <c r="X9" s="10">
-        <v>1287</v>
+      <c r="T9" s="27">
+        <v>1307</v>
+      </c>
+      <c r="U9" s="27">
+        <v>1308</v>
+      </c>
+      <c r="V9" s="27">
+        <v>1309</v>
+      </c>
+      <c r="W9" s="28">
+        <v>1309</v>
+      </c>
+      <c r="X9" s="27">
+        <v>1309</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
@@ -1148,67 +1181,67 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" si="0"/>
-        <v>526.54999999999995</v>
-      </c>
-      <c r="E10" s="6">
+        <v>528.29999999999995</v>
+      </c>
+      <c r="E10" s="20">
+        <v>511</v>
+      </c>
+      <c r="F10" s="20">
+        <v>514</v>
+      </c>
+      <c r="G10" s="20">
+        <v>515</v>
+      </c>
+      <c r="H10" s="20">
+        <v>515</v>
+      </c>
+      <c r="I10" s="20">
+        <v>515</v>
+      </c>
+      <c r="J10" s="6">
+        <v>516</v>
+      </c>
+      <c r="K10" s="6">
+        <v>517</v>
+      </c>
+      <c r="L10" s="6">
+        <v>519</v>
+      </c>
+      <c r="M10" s="6">
         <v>531</v>
       </c>
-      <c r="F10" s="6">
+      <c r="N10" s="6">
+        <v>532</v>
+      </c>
+      <c r="O10" s="6">
+        <v>533</v>
+      </c>
+      <c r="P10" s="6">
+        <v>533</v>
+      </c>
+      <c r="Q10" s="6">
         <v>534</v>
       </c>
-      <c r="G10" s="6">
-        <v>533</v>
-      </c>
-      <c r="H10" s="6">
-        <v>515</v>
-      </c>
-      <c r="I10" s="6">
+      <c r="R10" s="6">
         <v>534</v>
       </c>
-      <c r="J10" s="6">
+      <c r="S10" s="6">
         <v>534</v>
       </c>
-      <c r="K10" s="6">
+      <c r="T10" s="20">
         <v>534</v>
       </c>
-      <c r="L10" s="6">
-        <v>532</v>
-      </c>
-      <c r="M10" s="6">
-        <v>517</v>
-      </c>
-      <c r="N10" s="6">
-        <v>516</v>
-      </c>
-      <c r="O10" s="6">
+      <c r="U10" s="20">
+        <v>534</v>
+      </c>
+      <c r="V10" s="20">
+        <v>535</v>
+      </c>
+      <c r="W10" s="23">
+        <v>536</v>
+      </c>
+      <c r="X10" s="20">
         <v>539</v>
-      </c>
-      <c r="P10" s="6">
-        <v>515</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>533</v>
-      </c>
-      <c r="R10" s="6">
-        <v>535</v>
-      </c>
-      <c r="S10" s="6">
-        <v>511</v>
-      </c>
-      <c r="T10" s="6">
-        <v>514</v>
-      </c>
-      <c r="U10" s="6">
-        <v>515</v>
-      </c>
-      <c r="V10" s="6">
-        <v>534</v>
-      </c>
-      <c r="W10" s="5">
-        <v>536</v>
-      </c>
-      <c r="X10" s="6">
-        <v>519</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.3">
@@ -1220,67 +1253,67 @@
       </c>
       <c r="D11" s="3">
         <f t="shared" si="0"/>
-        <v>699.4</v>
-      </c>
-      <c r="E11" s="6">
+        <v>701.8</v>
+      </c>
+      <c r="E11" s="20">
+        <v>683</v>
+      </c>
+      <c r="F11" s="20">
+        <v>684</v>
+      </c>
+      <c r="G11" s="20">
+        <v>685</v>
+      </c>
+      <c r="H11" s="20">
+        <v>686</v>
+      </c>
+      <c r="I11" s="20">
+        <v>688</v>
+      </c>
+      <c r="J11" s="6">
+        <v>688</v>
+      </c>
+      <c r="K11" s="6">
+        <v>690</v>
+      </c>
+      <c r="L11" s="6">
+        <v>703</v>
+      </c>
+      <c r="M11" s="6">
+        <v>704</v>
+      </c>
+      <c r="N11" s="6">
+        <v>704</v>
+      </c>
+      <c r="O11" s="6">
+        <v>705</v>
+      </c>
+      <c r="P11" s="6">
         <v>706</v>
       </c>
-      <c r="F11" s="6">
+      <c r="Q11" s="6">
         <v>706</v>
       </c>
-      <c r="G11" s="6">
-        <v>704</v>
-      </c>
-      <c r="H11" s="6">
-        <v>686</v>
-      </c>
-      <c r="I11" s="6">
+      <c r="R11" s="6">
+        <v>706</v>
+      </c>
+      <c r="S11" s="6">
+        <v>706</v>
+      </c>
+      <c r="T11" s="20">
         <v>707</v>
       </c>
-      <c r="J11" s="6">
+      <c r="U11" s="20">
+        <v>708</v>
+      </c>
+      <c r="V11" s="20">
         <v>709</v>
       </c>
-      <c r="K11" s="6">
+      <c r="W11" s="23">
+        <v>709</v>
+      </c>
+      <c r="X11" s="20">
         <v>711</v>
-      </c>
-      <c r="L11" s="6">
-        <v>706</v>
-      </c>
-      <c r="M11" s="6">
-        <v>688</v>
-      </c>
-      <c r="N11" s="6">
-        <v>688</v>
-      </c>
-      <c r="O11" s="6">
-        <v>708</v>
-      </c>
-      <c r="P11" s="6">
-        <v>683</v>
-      </c>
-      <c r="Q11" s="6">
-        <v>703</v>
-      </c>
-      <c r="R11" s="6">
-        <v>709</v>
-      </c>
-      <c r="S11" s="6">
-        <v>684</v>
-      </c>
-      <c r="T11" s="6">
-        <v>704</v>
-      </c>
-      <c r="U11" s="6">
-        <v>685</v>
-      </c>
-      <c r="V11" s="6">
-        <v>705</v>
-      </c>
-      <c r="W11" s="5">
-        <v>706</v>
-      </c>
-      <c r="X11" s="6">
-        <v>690</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">
@@ -1292,67 +1325,67 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>1300.95</v>
-      </c>
-      <c r="E12" s="6">
+        <v>1303</v>
+      </c>
+      <c r="E12" s="20">
+        <v>1287</v>
+      </c>
+      <c r="F12" s="20">
+        <v>1288</v>
+      </c>
+      <c r="G12" s="20">
+        <v>1288</v>
+      </c>
+      <c r="H12" s="20">
+        <v>1288</v>
+      </c>
+      <c r="I12" s="20">
+        <v>1289</v>
+      </c>
+      <c r="J12" s="6">
+        <v>1289</v>
+      </c>
+      <c r="K12" s="6">
+        <v>1290</v>
+      </c>
+      <c r="L12" s="6">
+        <v>1303</v>
+      </c>
+      <c r="M12" s="6">
+        <v>1305</v>
+      </c>
+      <c r="N12" s="6">
         <v>1306</v>
       </c>
-      <c r="F12" s="6">
+      <c r="O12" s="6">
         <v>1307</v>
       </c>
-      <c r="G12" s="6">
-        <v>1305</v>
-      </c>
-      <c r="H12" s="6">
-        <v>1288</v>
-      </c>
-      <c r="I12" s="6">
+      <c r="P12" s="6">
+        <v>1307</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>1307</v>
+      </c>
+      <c r="R12" s="6">
         <v>1308</v>
       </c>
-      <c r="J12" s="6">
+      <c r="S12" s="6">
+        <v>1308</v>
+      </c>
+      <c r="T12" s="20">
         <v>1309</v>
       </c>
-      <c r="K12" s="6">
+      <c r="U12" s="20">
         <v>1309</v>
       </c>
-      <c r="L12" s="6">
+      <c r="V12" s="20">
         <v>1310</v>
       </c>
-      <c r="M12" s="6">
-        <v>1289</v>
-      </c>
-      <c r="N12" s="6">
-        <v>1289</v>
-      </c>
-      <c r="O12" s="6">
+      <c r="W12" s="23">
         <v>1310</v>
       </c>
-      <c r="P12" s="6">
-        <v>1288</v>
-      </c>
-      <c r="Q12" s="6">
-        <v>1303</v>
-      </c>
-      <c r="R12" s="6">
+      <c r="X12" s="20">
         <v>1311</v>
-      </c>
-      <c r="S12" s="6">
-        <v>1288</v>
-      </c>
-      <c r="T12" s="6">
-        <v>1307</v>
-      </c>
-      <c r="U12" s="6">
-        <v>1287</v>
-      </c>
-      <c r="V12" s="6">
-        <v>1307</v>
-      </c>
-      <c r="W12" s="5">
-        <v>1308</v>
-      </c>
-      <c r="X12" s="6">
-        <v>1290</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
@@ -1362,68 +1395,68 @@
       <c r="C13" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="3">
         <f t="shared" si="0"/>
-        <v>523.5</v>
-      </c>
-      <c r="E13" s="10">
-        <v>531</v>
-      </c>
-      <c r="F13" s="10">
-        <v>533</v>
-      </c>
-      <c r="G13" s="10">
-        <v>531</v>
-      </c>
-      <c r="H13" s="10">
-        <v>531</v>
-      </c>
-      <c r="I13" s="10">
-        <v>533</v>
+        <v>524</v>
+      </c>
+      <c r="E13" s="27">
+        <v>512</v>
+      </c>
+      <c r="F13" s="27">
+        <v>512</v>
+      </c>
+      <c r="G13" s="27">
+        <v>513</v>
+      </c>
+      <c r="H13" s="27">
+        <v>513</v>
+      </c>
+      <c r="I13" s="27">
+        <v>514</v>
       </c>
       <c r="J13" s="10">
-        <v>534</v>
+        <v>516</v>
       </c>
       <c r="K13" s="10">
-        <v>531</v>
+        <v>516</v>
       </c>
       <c r="L13" s="10">
         <v>516</v>
       </c>
       <c r="M13" s="10">
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="N13" s="10">
         <v>518</v>
       </c>
       <c r="O13" s="10">
-        <v>512</v>
+        <v>531</v>
       </c>
       <c r="P13" s="10">
-        <v>513</v>
+        <v>531</v>
       </c>
       <c r="Q13" s="10">
-        <v>514</v>
+        <v>531</v>
       </c>
       <c r="R13" s="10">
-        <v>512</v>
+        <v>531</v>
       </c>
       <c r="S13" s="10">
         <v>532</v>
       </c>
-      <c r="T13" s="10">
+      <c r="T13" s="20">
         <v>532</v>
       </c>
-      <c r="U13" s="10">
-        <v>516</v>
-      </c>
-      <c r="V13" s="10">
-        <v>518</v>
-      </c>
-      <c r="W13" s="8">
-        <v>516</v>
-      </c>
-      <c r="X13" s="10">
+      <c r="U13" s="20">
+        <v>533</v>
+      </c>
+      <c r="V13" s="20">
+        <v>533</v>
+      </c>
+      <c r="W13" s="23">
+        <v>534</v>
+      </c>
+      <c r="X13" s="20">
         <v>534</v>
       </c>
     </row>
@@ -1434,68 +1467,68 @@
       <c r="C14" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="3">
         <f t="shared" si="0"/>
-        <v>696.35</v>
-      </c>
-      <c r="E14" s="10">
+        <v>697.5</v>
+      </c>
+      <c r="E14" s="27">
+        <v>684</v>
+      </c>
+      <c r="F14" s="27">
+        <v>684</v>
+      </c>
+      <c r="G14" s="27">
+        <v>684</v>
+      </c>
+      <c r="H14" s="27">
+        <v>685</v>
+      </c>
+      <c r="I14" s="27">
+        <v>686</v>
+      </c>
+      <c r="J14" s="10">
+        <v>687</v>
+      </c>
+      <c r="K14" s="11">
+        <v>688</v>
+      </c>
+      <c r="L14" s="10">
+        <v>689</v>
+      </c>
+      <c r="M14" s="10">
+        <v>690</v>
+      </c>
+      <c r="N14" s="10">
+        <v>702</v>
+      </c>
+      <c r="O14" s="10">
         <v>703</v>
       </c>
-      <c r="F14" s="10">
-        <v>702</v>
-      </c>
-      <c r="G14" s="10">
+      <c r="P14" s="10">
+        <v>703</v>
+      </c>
+      <c r="Q14" s="10">
         <v>704</v>
       </c>
-      <c r="H14" s="10">
+      <c r="R14" s="10">
+        <v>704</v>
+      </c>
+      <c r="S14" s="10">
         <v>705</v>
       </c>
-      <c r="I14" s="10">
+      <c r="T14" s="20">
         <v>705</v>
       </c>
-      <c r="J14" s="10">
+      <c r="U14" s="20">
         <v>705</v>
       </c>
-      <c r="K14" s="11">
-        <v>703</v>
-      </c>
-      <c r="L14" s="10">
-        <v>688</v>
-      </c>
-      <c r="M14" s="10">
-        <v>684</v>
-      </c>
-      <c r="N14" s="10">
-        <v>686</v>
-      </c>
-      <c r="O14" s="10">
-        <v>684</v>
-      </c>
-      <c r="P14" s="10">
-        <v>685</v>
-      </c>
-      <c r="Q14" s="10">
-        <v>687</v>
-      </c>
-      <c r="R14" s="10">
-        <v>684</v>
-      </c>
-      <c r="S14" s="10">
-        <v>704</v>
-      </c>
-      <c r="T14" s="10">
+      <c r="V14" s="20">
         <v>706</v>
       </c>
-      <c r="U14" s="10">
-        <v>689</v>
-      </c>
-      <c r="V14" s="10">
+      <c r="W14" s="23">
         <v>706</v>
       </c>
-      <c r="W14" s="8">
-        <v>690</v>
-      </c>
-      <c r="X14" s="10">
+      <c r="X14" s="20">
         <v>707</v>
       </c>
     </row>
@@ -1506,69 +1539,69 @@
       <c r="C15" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="3">
         <f t="shared" si="0"/>
-        <v>1298.5999999999999</v>
-      </c>
-      <c r="E15" s="10">
-        <v>1308</v>
-      </c>
-      <c r="F15" s="10">
-        <v>1304</v>
-      </c>
-      <c r="G15" s="10">
-        <v>1307</v>
-      </c>
-      <c r="H15" s="10">
-        <v>1307</v>
-      </c>
-      <c r="I15" s="10">
-        <v>1308</v>
+        <v>1299.2</v>
+      </c>
+      <c r="E15" s="27">
+        <v>1287</v>
+      </c>
+      <c r="F15" s="27">
+        <v>1287</v>
+      </c>
+      <c r="G15" s="27">
+        <v>1288</v>
+      </c>
+      <c r="H15" s="27">
+        <v>1288</v>
+      </c>
+      <c r="I15" s="27">
+        <v>1289</v>
       </c>
       <c r="J15" s="10">
-        <v>1305</v>
+        <v>1290</v>
       </c>
       <c r="K15" s="10">
-        <v>1304</v>
+        <v>1290</v>
       </c>
       <c r="L15" s="10">
         <v>1290</v>
       </c>
       <c r="M15" s="10">
-        <v>1287</v>
+        <v>1291</v>
       </c>
       <c r="N15" s="10">
-        <v>1290</v>
+        <v>1304</v>
       </c>
       <c r="O15" s="10">
-        <v>1288</v>
+        <v>1304</v>
       </c>
       <c r="P15" s="10">
-        <v>1287</v>
+        <v>1304</v>
       </c>
       <c r="Q15" s="10">
-        <v>1288</v>
+        <v>1305</v>
       </c>
       <c r="R15" s="10">
-        <v>1289</v>
+        <v>1307</v>
       </c>
       <c r="S15" s="10">
-        <v>1304</v>
-      </c>
-      <c r="T15" s="10">
         <v>1307</v>
       </c>
-      <c r="U15" s="10">
-        <v>1291</v>
-      </c>
-      <c r="V15" s="10">
+      <c r="T15" s="20">
+        <v>1307</v>
+      </c>
+      <c r="U15" s="20">
+        <v>1308</v>
+      </c>
+      <c r="V15" s="20">
+        <v>1308</v>
+      </c>
+      <c r="W15" s="23">
+        <v>1308</v>
+      </c>
+      <c r="X15" s="20">
         <v>1310</v>
-      </c>
-      <c r="W15" s="8">
-        <v>1290</v>
-      </c>
-      <c r="X15" s="10">
-        <v>1308</v>
       </c>
     </row>
     <row r="17" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1586,19 +1619,19 @@
       <c r="D18" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="24">
         <v>1</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="24">
         <v>2</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="24">
         <v>3</v>
       </c>
-      <c r="H18" s="17">
+      <c r="H18" s="24">
         <v>4</v>
       </c>
-      <c r="I18" s="17">
+      <c r="I18" s="24">
         <v>5</v>
       </c>
       <c r="J18" s="17">
@@ -1631,19 +1664,19 @@
       <c r="S18" s="17">
         <v>15</v>
       </c>
-      <c r="T18" s="17">
+      <c r="T18" s="24">
         <v>16</v>
       </c>
-      <c r="U18" s="17">
+      <c r="U18" s="24">
         <v>17</v>
       </c>
-      <c r="V18" s="17">
+      <c r="V18" s="24">
         <v>18</v>
       </c>
-      <c r="W18" s="16">
+      <c r="W18" s="25">
         <v>19</v>
       </c>
-      <c r="X18" s="17">
+      <c r="X18" s="24">
         <v>20</v>
       </c>
     </row>
@@ -1655,22 +1688,22 @@
         <v>1</v>
       </c>
       <c r="D19" s="3">
-        <f>AVERAGE(E19:AC19)</f>
-        <v>261</v>
-      </c>
-      <c r="E19" s="3">
-        <v>261</v>
-      </c>
-      <c r="F19" s="3">
-        <v>261</v>
-      </c>
-      <c r="G19" s="3">
-        <v>261</v>
-      </c>
-      <c r="H19" s="3">
-        <v>261</v>
-      </c>
-      <c r="I19" s="3">
+        <f>AVERAGE(J19:S19)</f>
+        <v>261</v>
+      </c>
+      <c r="E19" s="19">
+        <v>261</v>
+      </c>
+      <c r="F19" s="19">
+        <v>261</v>
+      </c>
+      <c r="G19" s="19">
+        <v>261</v>
+      </c>
+      <c r="H19" s="19">
+        <v>261</v>
+      </c>
+      <c r="I19" s="19">
         <v>261</v>
       </c>
       <c r="J19" s="3">
@@ -1703,19 +1736,19 @@
       <c r="S19" s="3">
         <v>261</v>
       </c>
-      <c r="T19" s="3">
-        <v>261</v>
-      </c>
-      <c r="U19" s="3">
-        <v>261</v>
-      </c>
-      <c r="V19" s="3">
-        <v>261</v>
-      </c>
-      <c r="W19" s="3">
-        <v>261</v>
-      </c>
-      <c r="X19" s="3">
+      <c r="T19" s="19">
+        <v>261</v>
+      </c>
+      <c r="U19" s="19">
+        <v>261</v>
+      </c>
+      <c r="V19" s="19">
+        <v>261</v>
+      </c>
+      <c r="W19" s="19">
+        <v>261</v>
+      </c>
+      <c r="X19" s="19">
         <v>261</v>
       </c>
     </row>
@@ -1727,22 +1760,22 @@
         <v>2</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" ref="D20:D30" si="1">AVERAGE(E20:AC20)</f>
-        <v>477</v>
-      </c>
-      <c r="E20" s="3">
-        <v>477</v>
-      </c>
-      <c r="F20" s="3">
-        <v>477</v>
-      </c>
-      <c r="G20" s="3">
-        <v>477</v>
-      </c>
-      <c r="H20" s="3">
-        <v>477</v>
-      </c>
-      <c r="I20" s="3">
+        <f t="shared" ref="D20:D30" si="1">AVERAGE(J20:S20)</f>
+        <v>477</v>
+      </c>
+      <c r="E20" s="19">
+        <v>477</v>
+      </c>
+      <c r="F20" s="19">
+        <v>477</v>
+      </c>
+      <c r="G20" s="19">
+        <v>477</v>
+      </c>
+      <c r="H20" s="19">
+        <v>477</v>
+      </c>
+      <c r="I20" s="19">
         <v>477</v>
       </c>
       <c r="J20" s="3">
@@ -1775,19 +1808,19 @@
       <c r="S20" s="3">
         <v>477</v>
       </c>
-      <c r="T20" s="3">
-        <v>477</v>
-      </c>
-      <c r="U20" s="3">
-        <v>477</v>
-      </c>
-      <c r="V20" s="3">
-        <v>477</v>
-      </c>
-      <c r="W20" s="3">
-        <v>477</v>
-      </c>
-      <c r="X20" s="3">
+      <c r="T20" s="19">
+        <v>477</v>
+      </c>
+      <c r="U20" s="19">
+        <v>477</v>
+      </c>
+      <c r="V20" s="19">
+        <v>477</v>
+      </c>
+      <c r="W20" s="19">
+        <v>477</v>
+      </c>
+      <c r="X20" s="19">
         <v>477</v>
       </c>
     </row>
@@ -1802,19 +1835,19 @@
         <f t="shared" si="1"/>
         <v>1331</v>
       </c>
-      <c r="E21" s="3">
-        <v>1331</v>
-      </c>
-      <c r="F21" s="3">
-        <v>1331</v>
-      </c>
-      <c r="G21" s="3">
-        <v>1331</v>
-      </c>
-      <c r="H21" s="3">
-        <v>1331</v>
-      </c>
-      <c r="I21" s="3">
+      <c r="E21" s="19">
+        <v>1331</v>
+      </c>
+      <c r="F21" s="19">
+        <v>1331</v>
+      </c>
+      <c r="G21" s="19">
+        <v>1331</v>
+      </c>
+      <c r="H21" s="19">
+        <v>1331</v>
+      </c>
+      <c r="I21" s="19">
         <v>1331</v>
       </c>
       <c r="J21" s="3">
@@ -1847,19 +1880,19 @@
       <c r="S21" s="3">
         <v>1331</v>
       </c>
-      <c r="T21" s="3">
-        <v>1331</v>
-      </c>
-      <c r="U21" s="3">
-        <v>1331</v>
-      </c>
-      <c r="V21" s="3">
-        <v>1331</v>
-      </c>
-      <c r="W21" s="3">
-        <v>1331</v>
-      </c>
-      <c r="X21" s="3">
+      <c r="T21" s="19">
+        <v>1331</v>
+      </c>
+      <c r="U21" s="19">
+        <v>1331</v>
+      </c>
+      <c r="V21" s="19">
+        <v>1331</v>
+      </c>
+      <c r="W21" s="19">
+        <v>1331</v>
+      </c>
+      <c r="X21" s="19">
         <v>1331</v>
       </c>
     </row>
@@ -1870,23 +1903,23 @@
       <c r="C22" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="3">
         <f t="shared" si="1"/>
         <v>261</v>
       </c>
-      <c r="E22" s="9">
-        <v>261</v>
-      </c>
-      <c r="F22" s="9">
-        <v>261</v>
-      </c>
-      <c r="G22" s="9">
-        <v>261</v>
-      </c>
-      <c r="H22" s="9">
-        <v>261</v>
-      </c>
-      <c r="I22" s="9">
+      <c r="E22" s="26">
+        <v>261</v>
+      </c>
+      <c r="F22" s="26">
+        <v>261</v>
+      </c>
+      <c r="G22" s="26">
+        <v>261</v>
+      </c>
+      <c r="H22" s="26">
+        <v>261</v>
+      </c>
+      <c r="I22" s="26">
         <v>261</v>
       </c>
       <c r="J22" s="9">
@@ -1919,19 +1952,19 @@
       <c r="S22" s="9">
         <v>261</v>
       </c>
-      <c r="T22" s="9">
-        <v>261</v>
-      </c>
-      <c r="U22" s="9">
-        <v>261</v>
-      </c>
-      <c r="V22" s="9">
-        <v>261</v>
-      </c>
-      <c r="W22" s="9">
-        <v>261</v>
-      </c>
-      <c r="X22" s="9">
+      <c r="T22" s="26">
+        <v>261</v>
+      </c>
+      <c r="U22" s="26">
+        <v>261</v>
+      </c>
+      <c r="V22" s="26">
+        <v>261</v>
+      </c>
+      <c r="W22" s="26">
+        <v>261</v>
+      </c>
+      <c r="X22" s="26">
         <v>261</v>
       </c>
     </row>
@@ -1942,23 +1975,23 @@
       <c r="C23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="3">
         <f t="shared" si="1"/>
         <v>477</v>
       </c>
-      <c r="E23" s="9">
-        <v>477</v>
-      </c>
-      <c r="F23" s="9">
-        <v>477</v>
-      </c>
-      <c r="G23" s="9">
-        <v>477</v>
-      </c>
-      <c r="H23" s="9">
-        <v>477</v>
-      </c>
-      <c r="I23" s="9">
+      <c r="E23" s="26">
+        <v>477</v>
+      </c>
+      <c r="F23" s="26">
+        <v>477</v>
+      </c>
+      <c r="G23" s="26">
+        <v>477</v>
+      </c>
+      <c r="H23" s="26">
+        <v>477</v>
+      </c>
+      <c r="I23" s="26">
         <v>477</v>
       </c>
       <c r="J23" s="9">
@@ -1991,19 +2024,19 @@
       <c r="S23" s="9">
         <v>477</v>
       </c>
-      <c r="T23" s="9">
-        <v>477</v>
-      </c>
-      <c r="U23" s="9">
-        <v>477</v>
-      </c>
-      <c r="V23" s="9">
-        <v>477</v>
-      </c>
-      <c r="W23" s="9">
-        <v>477</v>
-      </c>
-      <c r="X23" s="9">
+      <c r="T23" s="26">
+        <v>477</v>
+      </c>
+      <c r="U23" s="26">
+        <v>477</v>
+      </c>
+      <c r="V23" s="26">
+        <v>477</v>
+      </c>
+      <c r="W23" s="26">
+        <v>477</v>
+      </c>
+      <c r="X23" s="26">
         <v>477</v>
       </c>
     </row>
@@ -2014,23 +2047,23 @@
       <c r="C24" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="3">
         <f t="shared" si="1"/>
         <v>1331</v>
       </c>
-      <c r="E24" s="9">
-        <v>1331</v>
-      </c>
-      <c r="F24" s="9">
-        <v>1331</v>
-      </c>
-      <c r="G24" s="9">
-        <v>1331</v>
-      </c>
-      <c r="H24" s="9">
-        <v>1331</v>
-      </c>
-      <c r="I24" s="9">
+      <c r="E24" s="26">
+        <v>1331</v>
+      </c>
+      <c r="F24" s="26">
+        <v>1331</v>
+      </c>
+      <c r="G24" s="26">
+        <v>1331</v>
+      </c>
+      <c r="H24" s="26">
+        <v>1331</v>
+      </c>
+      <c r="I24" s="26">
         <v>1331</v>
       </c>
       <c r="J24" s="9">
@@ -2063,19 +2096,19 @@
       <c r="S24" s="9">
         <v>1331</v>
       </c>
-      <c r="T24" s="9">
-        <v>1331</v>
-      </c>
-      <c r="U24" s="9">
-        <v>1331</v>
-      </c>
-      <c r="V24" s="9">
-        <v>1331</v>
-      </c>
-      <c r="W24" s="9">
-        <v>1331</v>
-      </c>
-      <c r="X24" s="9">
+      <c r="T24" s="26">
+        <v>1331</v>
+      </c>
+      <c r="U24" s="26">
+        <v>1331</v>
+      </c>
+      <c r="V24" s="26">
+        <v>1331</v>
+      </c>
+      <c r="W24" s="26">
+        <v>1331</v>
+      </c>
+      <c r="X24" s="26">
         <v>1331</v>
       </c>
     </row>
@@ -2090,19 +2123,19 @@
         <f t="shared" si="1"/>
         <v>261</v>
       </c>
-      <c r="E25" s="3">
-        <v>261</v>
-      </c>
-      <c r="F25" s="3">
-        <v>261</v>
-      </c>
-      <c r="G25" s="3">
-        <v>261</v>
-      </c>
-      <c r="H25" s="3">
-        <v>261</v>
-      </c>
-      <c r="I25" s="3">
+      <c r="E25" s="19">
+        <v>261</v>
+      </c>
+      <c r="F25" s="19">
+        <v>261</v>
+      </c>
+      <c r="G25" s="19">
+        <v>261</v>
+      </c>
+      <c r="H25" s="19">
+        <v>261</v>
+      </c>
+      <c r="I25" s="19">
         <v>261</v>
       </c>
       <c r="J25" s="3">
@@ -2135,19 +2168,19 @@
       <c r="S25" s="3">
         <v>261</v>
       </c>
-      <c r="T25" s="3">
-        <v>261</v>
-      </c>
-      <c r="U25" s="3">
-        <v>261</v>
-      </c>
-      <c r="V25" s="3">
-        <v>261</v>
-      </c>
-      <c r="W25" s="3">
-        <v>261</v>
-      </c>
-      <c r="X25" s="3">
+      <c r="T25" s="19">
+        <v>261</v>
+      </c>
+      <c r="U25" s="19">
+        <v>261</v>
+      </c>
+      <c r="V25" s="19">
+        <v>261</v>
+      </c>
+      <c r="W25" s="19">
+        <v>261</v>
+      </c>
+      <c r="X25" s="19">
         <v>261</v>
       </c>
     </row>
@@ -2162,19 +2195,19 @@
         <f t="shared" si="1"/>
         <v>477</v>
       </c>
-      <c r="E26" s="3">
-        <v>477</v>
-      </c>
-      <c r="F26" s="3">
-        <v>477</v>
-      </c>
-      <c r="G26" s="3">
-        <v>477</v>
-      </c>
-      <c r="H26" s="3">
-        <v>477</v>
-      </c>
-      <c r="I26" s="3">
+      <c r="E26" s="19">
+        <v>477</v>
+      </c>
+      <c r="F26" s="19">
+        <v>477</v>
+      </c>
+      <c r="G26" s="19">
+        <v>477</v>
+      </c>
+      <c r="H26" s="19">
+        <v>477</v>
+      </c>
+      <c r="I26" s="19">
         <v>477</v>
       </c>
       <c r="J26" s="3">
@@ -2207,19 +2240,19 @@
       <c r="S26" s="3">
         <v>477</v>
       </c>
-      <c r="T26" s="3">
-        <v>477</v>
-      </c>
-      <c r="U26" s="3">
-        <v>477</v>
-      </c>
-      <c r="V26" s="3">
-        <v>477</v>
-      </c>
-      <c r="W26" s="3">
-        <v>477</v>
-      </c>
-      <c r="X26" s="3">
+      <c r="T26" s="19">
+        <v>477</v>
+      </c>
+      <c r="U26" s="19">
+        <v>477</v>
+      </c>
+      <c r="V26" s="19">
+        <v>477</v>
+      </c>
+      <c r="W26" s="19">
+        <v>477</v>
+      </c>
+      <c r="X26" s="19">
         <v>477</v>
       </c>
     </row>
@@ -2234,19 +2267,19 @@
         <f t="shared" si="1"/>
         <v>1331</v>
       </c>
-      <c r="E27" s="3">
-        <v>1331</v>
-      </c>
-      <c r="F27" s="3">
-        <v>1331</v>
-      </c>
-      <c r="G27" s="3">
-        <v>1331</v>
-      </c>
-      <c r="H27" s="3">
-        <v>1331</v>
-      </c>
-      <c r="I27" s="3">
+      <c r="E27" s="19">
+        <v>1331</v>
+      </c>
+      <c r="F27" s="19">
+        <v>1331</v>
+      </c>
+      <c r="G27" s="19">
+        <v>1331</v>
+      </c>
+      <c r="H27" s="19">
+        <v>1331</v>
+      </c>
+      <c r="I27" s="19">
         <v>1331</v>
       </c>
       <c r="J27" s="3">
@@ -2279,19 +2312,19 @@
       <c r="S27" s="3">
         <v>1331</v>
       </c>
-      <c r="T27" s="3">
-        <v>1331</v>
-      </c>
-      <c r="U27" s="3">
-        <v>1331</v>
-      </c>
-      <c r="V27" s="3">
-        <v>1331</v>
-      </c>
-      <c r="W27" s="3">
-        <v>1331</v>
-      </c>
-      <c r="X27" s="3">
+      <c r="T27" s="19">
+        <v>1331</v>
+      </c>
+      <c r="U27" s="19">
+        <v>1331</v>
+      </c>
+      <c r="V27" s="19">
+        <v>1331</v>
+      </c>
+      <c r="W27" s="19">
+        <v>1331</v>
+      </c>
+      <c r="X27" s="19">
         <v>1331</v>
       </c>
     </row>
@@ -2302,23 +2335,23 @@
       <c r="C28" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="9">
-        <f>AVERAGE(E28:AC28)</f>
-        <v>261</v>
-      </c>
-      <c r="E28" s="9">
-        <v>261</v>
-      </c>
-      <c r="F28" s="9">
-        <v>261</v>
-      </c>
-      <c r="G28" s="9">
-        <v>261</v>
-      </c>
-      <c r="H28" s="9">
-        <v>261</v>
-      </c>
-      <c r="I28" s="9">
+      <c r="D28" s="3">
+        <f t="shared" si="1"/>
+        <v>261</v>
+      </c>
+      <c r="E28" s="26">
+        <v>261</v>
+      </c>
+      <c r="F28" s="26">
+        <v>261</v>
+      </c>
+      <c r="G28" s="26">
+        <v>261</v>
+      </c>
+      <c r="H28" s="26">
+        <v>261</v>
+      </c>
+      <c r="I28" s="26">
         <v>261</v>
       </c>
       <c r="J28" s="9">
@@ -2351,19 +2384,19 @@
       <c r="S28" s="9">
         <v>261</v>
       </c>
-      <c r="T28" s="9">
-        <v>261</v>
-      </c>
-      <c r="U28" s="9">
-        <v>261</v>
-      </c>
-      <c r="V28" s="9">
-        <v>261</v>
-      </c>
-      <c r="W28" s="9">
-        <v>261</v>
-      </c>
-      <c r="X28" s="9">
+      <c r="T28" s="26">
+        <v>261</v>
+      </c>
+      <c r="U28" s="26">
+        <v>261</v>
+      </c>
+      <c r="V28" s="26">
+        <v>261</v>
+      </c>
+      <c r="W28" s="26">
+        <v>261</v>
+      </c>
+      <c r="X28" s="26">
         <v>261</v>
       </c>
     </row>
@@ -2374,23 +2407,23 @@
       <c r="C29" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="3">
         <f t="shared" si="1"/>
         <v>477</v>
       </c>
-      <c r="E29" s="9">
-        <v>477</v>
-      </c>
-      <c r="F29" s="9">
-        <v>477</v>
-      </c>
-      <c r="G29" s="9">
-        <v>477</v>
-      </c>
-      <c r="H29" s="9">
-        <v>477</v>
-      </c>
-      <c r="I29" s="9">
+      <c r="E29" s="26">
+        <v>477</v>
+      </c>
+      <c r="F29" s="26">
+        <v>477</v>
+      </c>
+      <c r="G29" s="26">
+        <v>477</v>
+      </c>
+      <c r="H29" s="26">
+        <v>477</v>
+      </c>
+      <c r="I29" s="26">
         <v>477</v>
       </c>
       <c r="J29" s="9">
@@ -2423,19 +2456,19 @@
       <c r="S29" s="9">
         <v>477</v>
       </c>
-      <c r="T29" s="9">
-        <v>477</v>
-      </c>
-      <c r="U29" s="9">
-        <v>477</v>
-      </c>
-      <c r="V29" s="9">
-        <v>477</v>
-      </c>
-      <c r="W29" s="9">
-        <v>477</v>
-      </c>
-      <c r="X29" s="9">
+      <c r="T29" s="26">
+        <v>477</v>
+      </c>
+      <c r="U29" s="26">
+        <v>477</v>
+      </c>
+      <c r="V29" s="26">
+        <v>477</v>
+      </c>
+      <c r="W29" s="26">
+        <v>477</v>
+      </c>
+      <c r="X29" s="26">
         <v>477</v>
       </c>
     </row>
@@ -2446,23 +2479,23 @@
       <c r="C30" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="3">
         <f t="shared" si="1"/>
         <v>1331</v>
       </c>
-      <c r="E30" s="9">
-        <v>1331</v>
-      </c>
-      <c r="F30" s="9">
-        <v>1331</v>
-      </c>
-      <c r="G30" s="9">
-        <v>1331</v>
-      </c>
-      <c r="H30" s="9">
-        <v>1331</v>
-      </c>
-      <c r="I30" s="9">
+      <c r="E30" s="26">
+        <v>1331</v>
+      </c>
+      <c r="F30" s="26">
+        <v>1331</v>
+      </c>
+      <c r="G30" s="26">
+        <v>1331</v>
+      </c>
+      <c r="H30" s="26">
+        <v>1331</v>
+      </c>
+      <c r="I30" s="26">
         <v>1331</v>
       </c>
       <c r="J30" s="9">
@@ -2495,23 +2528,26 @@
       <c r="S30" s="9">
         <v>1331</v>
       </c>
-      <c r="T30" s="9">
-        <v>1331</v>
-      </c>
-      <c r="U30" s="9">
-        <v>1331</v>
-      </c>
-      <c r="V30" s="9">
-        <v>1331</v>
-      </c>
-      <c r="W30" s="9">
-        <v>1331</v>
-      </c>
-      <c r="X30" s="9">
+      <c r="T30" s="26">
+        <v>1331</v>
+      </c>
+      <c r="U30" s="26">
+        <v>1331</v>
+      </c>
+      <c r="V30" s="26">
+        <v>1331</v>
+      </c>
+      <c r="W30" s="26">
+        <v>1331</v>
+      </c>
+      <c r="X30" s="26">
         <v>1331</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="E15:X15">
+    <sortCondition ref="E15:X15"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Sorted HBAO memory measurements
</commit_message>
<xml_diff>
--- a/Experiment/Results/MemoryUsageSorted.xlsx
+++ b/Experiment/Results/MemoryUsageSorted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Howest\GD_J3_S2\Gradwork_2.0\Gradwork\Experiment\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F615D0E2-6CA5-4C60-BF6D-C2E36107C3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91E80E0-0573-4F90-AF21-3C1809B77ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10790" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-10790" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SSAO" sheetId="1" r:id="rId1"/>
@@ -353,7 +353,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyBorder="1"/>
@@ -364,6 +363,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="4" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent2" xfId="4" builtinId="34"/>
@@ -652,7 +652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -679,19 +679,19 @@
       <c r="D3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="23">
         <v>1</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="23">
         <v>2</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="23">
         <v>3</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="23">
         <v>4</v>
       </c>
-      <c r="I3" s="24">
+      <c r="I3" s="23">
         <v>5</v>
       </c>
       <c r="J3" s="17">
@@ -724,19 +724,19 @@
       <c r="S3" s="17">
         <v>15</v>
       </c>
-      <c r="T3" s="24">
+      <c r="T3" s="23">
         <v>16</v>
       </c>
-      <c r="U3" s="24">
+      <c r="U3" s="23">
         <v>17</v>
       </c>
-      <c r="V3" s="24">
+      <c r="V3" s="23">
         <v>18</v>
       </c>
-      <c r="W3" s="25">
+      <c r="W3" s="24">
         <v>19</v>
       </c>
-      <c r="X3" s="24">
+      <c r="X3" s="23">
         <v>20</v>
       </c>
     </row>
@@ -751,19 +751,19 @@
         <f>AVERAGE(J4:S4)</f>
         <v>514.9</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="18">
         <v>511</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="18">
         <v>512</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="18">
         <v>512</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="18">
         <v>512</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="18">
         <v>513</v>
       </c>
       <c r="J4" s="3">
@@ -796,19 +796,19 @@
       <c r="S4" s="3">
         <v>516</v>
       </c>
-      <c r="T4" s="19">
+      <c r="T4" s="18">
         <v>517</v>
       </c>
-      <c r="U4" s="19">
+      <c r="U4" s="18">
         <v>517</v>
       </c>
-      <c r="V4" s="21">
+      <c r="V4" s="20">
         <v>517</v>
       </c>
-      <c r="W4" s="22">
+      <c r="W4" s="21">
         <v>518</v>
       </c>
-      <c r="X4" s="19">
+      <c r="X4" s="18">
         <v>518</v>
       </c>
     </row>
@@ -823,19 +823,19 @@
         <f t="shared" ref="D5:D15" si="0">AVERAGE(J5:S5)</f>
         <v>687.1</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="19">
         <v>684</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="19">
         <v>684</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="19">
         <v>685</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="19">
         <v>685</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="19">
         <v>686</v>
       </c>
       <c r="J5" s="6">
@@ -868,19 +868,19 @@
       <c r="S5" s="6">
         <v>690</v>
       </c>
-      <c r="T5" s="20">
+      <c r="T5" s="19">
         <v>690</v>
       </c>
-      <c r="U5" s="20">
+      <c r="U5" s="19">
         <v>693</v>
       </c>
-      <c r="V5" s="20">
+      <c r="V5" s="19">
         <v>703</v>
       </c>
-      <c r="W5" s="23">
+      <c r="W5" s="22">
         <v>703</v>
       </c>
-      <c r="X5" s="20">
+      <c r="X5" s="19">
         <v>708</v>
       </c>
     </row>
@@ -895,19 +895,19 @@
         <f t="shared" si="0"/>
         <v>1290</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="19">
         <v>1287</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="19">
         <v>1287</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="19">
         <v>1288</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="19">
         <v>1288</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="19">
         <v>1288</v>
       </c>
       <c r="J6" s="6">
@@ -940,19 +940,19 @@
       <c r="S6" s="6">
         <v>1293</v>
       </c>
-      <c r="T6" s="20">
+      <c r="T6" s="19">
         <v>1304</v>
       </c>
-      <c r="U6" s="20">
+      <c r="U6" s="19">
         <v>1305</v>
       </c>
-      <c r="V6" s="20">
+      <c r="V6" s="19">
         <v>1306</v>
       </c>
-      <c r="W6" s="23">
+      <c r="W6" s="22">
         <v>1307</v>
       </c>
-      <c r="X6" s="20">
+      <c r="X6" s="19">
         <v>1309</v>
       </c>
     </row>
@@ -967,19 +967,19 @@
         <f t="shared" si="0"/>
         <v>514.70000000000005</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <v>511</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="26">
         <v>512</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7" s="26">
         <v>513</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="26">
         <v>513</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7" s="26">
         <v>514</v>
       </c>
       <c r="J7" s="10">
@@ -1012,19 +1012,19 @@
       <c r="S7" s="10">
         <v>516</v>
       </c>
-      <c r="T7" s="27">
+      <c r="T7" s="26">
         <v>516</v>
       </c>
-      <c r="U7" s="27">
+      <c r="U7" s="26">
         <v>517</v>
       </c>
-      <c r="V7" s="27">
+      <c r="V7" s="26">
         <v>532</v>
       </c>
-      <c r="W7" s="28">
+      <c r="W7" s="27">
         <v>533</v>
       </c>
-      <c r="X7" s="27">
+      <c r="X7" s="26">
         <v>539</v>
       </c>
     </row>
@@ -1039,19 +1039,19 @@
         <f t="shared" si="0"/>
         <v>702.1</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="26">
         <v>683</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="26">
         <v>684</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="26">
         <v>686</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="26">
         <v>686</v>
       </c>
-      <c r="I8" s="27">
+      <c r="I8" s="26">
         <v>686</v>
       </c>
       <c r="J8" s="10">
@@ -1084,19 +1084,19 @@
       <c r="S8" s="10">
         <v>706</v>
       </c>
-      <c r="T8" s="27">
+      <c r="T8" s="26">
         <v>706</v>
       </c>
-      <c r="U8" s="27">
+      <c r="U8" s="26">
         <v>706</v>
       </c>
-      <c r="V8" s="27">
+      <c r="V8" s="26">
         <v>706</v>
       </c>
-      <c r="W8" s="28">
+      <c r="W8" s="27">
         <v>707</v>
       </c>
-      <c r="X8" s="27">
+      <c r="X8" s="26">
         <v>710</v>
       </c>
     </row>
@@ -1111,19 +1111,19 @@
         <f t="shared" si="0"/>
         <v>1306.0999999999999</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="26">
         <v>1287</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="26">
         <v>1288</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="26">
         <v>1289</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="26">
         <v>1291</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="26">
         <v>1305</v>
       </c>
       <c r="J9" s="10">
@@ -1156,19 +1156,19 @@
       <c r="S9" s="10">
         <v>1307</v>
       </c>
-      <c r="T9" s="27">
+      <c r="T9" s="26">
         <v>1307</v>
       </c>
-      <c r="U9" s="27">
+      <c r="U9" s="26">
         <v>1308</v>
       </c>
-      <c r="V9" s="27">
+      <c r="V9" s="26">
         <v>1309</v>
       </c>
-      <c r="W9" s="28">
+      <c r="W9" s="27">
         <v>1309</v>
       </c>
-      <c r="X9" s="27">
+      <c r="X9" s="26">
         <v>1309</v>
       </c>
     </row>
@@ -1183,19 +1183,19 @@
         <f t="shared" si="0"/>
         <v>528.29999999999995</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="19">
         <v>511</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="19">
         <v>514</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="19">
         <v>515</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="19">
         <v>515</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="19">
         <v>515</v>
       </c>
       <c r="J10" s="6">
@@ -1228,19 +1228,19 @@
       <c r="S10" s="6">
         <v>534</v>
       </c>
-      <c r="T10" s="20">
+      <c r="T10" s="19">
         <v>534</v>
       </c>
-      <c r="U10" s="20">
+      <c r="U10" s="19">
         <v>534</v>
       </c>
-      <c r="V10" s="20">
+      <c r="V10" s="19">
         <v>535</v>
       </c>
-      <c r="W10" s="23">
+      <c r="W10" s="22">
         <v>536</v>
       </c>
-      <c r="X10" s="20">
+      <c r="X10" s="19">
         <v>539</v>
       </c>
     </row>
@@ -1255,19 +1255,19 @@
         <f t="shared" si="0"/>
         <v>701.8</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="19">
         <v>683</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="19">
         <v>684</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="19">
         <v>685</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="19">
         <v>686</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="19">
         <v>688</v>
       </c>
       <c r="J11" s="6">
@@ -1300,19 +1300,19 @@
       <c r="S11" s="6">
         <v>706</v>
       </c>
-      <c r="T11" s="20">
+      <c r="T11" s="19">
         <v>707</v>
       </c>
-      <c r="U11" s="20">
+      <c r="U11" s="19">
         <v>708</v>
       </c>
-      <c r="V11" s="20">
+      <c r="V11" s="19">
         <v>709</v>
       </c>
-      <c r="W11" s="23">
+      <c r="W11" s="22">
         <v>709</v>
       </c>
-      <c r="X11" s="20">
+      <c r="X11" s="19">
         <v>711</v>
       </c>
     </row>
@@ -1327,19 +1327,19 @@
         <f t="shared" si="0"/>
         <v>1303</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="19">
         <v>1287</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="19">
         <v>1288</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="19">
         <v>1288</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="19">
         <v>1288</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="19">
         <v>1289</v>
       </c>
       <c r="J12" s="6">
@@ -1372,19 +1372,19 @@
       <c r="S12" s="6">
         <v>1308</v>
       </c>
-      <c r="T12" s="20">
+      <c r="T12" s="19">
         <v>1309</v>
       </c>
-      <c r="U12" s="20">
+      <c r="U12" s="19">
         <v>1309</v>
       </c>
-      <c r="V12" s="20">
+      <c r="V12" s="19">
         <v>1310</v>
       </c>
-      <c r="W12" s="23">
+      <c r="W12" s="22">
         <v>1310</v>
       </c>
-      <c r="X12" s="20">
+      <c r="X12" s="19">
         <v>1311</v>
       </c>
     </row>
@@ -1399,19 +1399,19 @@
         <f t="shared" si="0"/>
         <v>524</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="26">
         <v>512</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="26">
         <v>512</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="26">
         <v>513</v>
       </c>
-      <c r="H13" s="27">
+      <c r="H13" s="26">
         <v>513</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I13" s="26">
         <v>514</v>
       </c>
       <c r="J13" s="10">
@@ -1444,19 +1444,19 @@
       <c r="S13" s="10">
         <v>532</v>
       </c>
-      <c r="T13" s="20">
+      <c r="T13" s="19">
         <v>532</v>
       </c>
-      <c r="U13" s="20">
+      <c r="U13" s="19">
         <v>533</v>
       </c>
-      <c r="V13" s="20">
+      <c r="V13" s="19">
         <v>533</v>
       </c>
-      <c r="W13" s="23">
+      <c r="W13" s="22">
         <v>534</v>
       </c>
-      <c r="X13" s="20">
+      <c r="X13" s="19">
         <v>534</v>
       </c>
     </row>
@@ -1471,19 +1471,19 @@
         <f t="shared" si="0"/>
         <v>697.5</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="26">
         <v>684</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="26">
         <v>684</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="26">
         <v>684</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H14" s="26">
         <v>685</v>
       </c>
-      <c r="I14" s="27">
+      <c r="I14" s="26">
         <v>686</v>
       </c>
       <c r="J14" s="10">
@@ -1516,19 +1516,19 @@
       <c r="S14" s="10">
         <v>705</v>
       </c>
-      <c r="T14" s="20">
+      <c r="T14" s="19">
         <v>705</v>
       </c>
-      <c r="U14" s="20">
+      <c r="U14" s="19">
         <v>705</v>
       </c>
-      <c r="V14" s="20">
+      <c r="V14" s="19">
         <v>706</v>
       </c>
-      <c r="W14" s="23">
+      <c r="W14" s="22">
         <v>706</v>
       </c>
-      <c r="X14" s="20">
+      <c r="X14" s="19">
         <v>707</v>
       </c>
     </row>
@@ -1543,19 +1543,19 @@
         <f t="shared" si="0"/>
         <v>1299.2</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="26">
         <v>1287</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="26">
         <v>1287</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="26">
         <v>1288</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H15" s="26">
         <v>1288</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I15" s="26">
         <v>1289</v>
       </c>
       <c r="J15" s="10">
@@ -1588,19 +1588,19 @@
       <c r="S15" s="10">
         <v>1307</v>
       </c>
-      <c r="T15" s="20">
+      <c r="T15" s="19">
         <v>1307</v>
       </c>
-      <c r="U15" s="20">
+      <c r="U15" s="19">
         <v>1308</v>
       </c>
-      <c r="V15" s="20">
+      <c r="V15" s="19">
         <v>1308</v>
       </c>
-      <c r="W15" s="23">
+      <c r="W15" s="22">
         <v>1308</v>
       </c>
-      <c r="X15" s="20">
+      <c r="X15" s="19">
         <v>1310</v>
       </c>
     </row>
@@ -1619,19 +1619,19 @@
       <c r="D18" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="23">
         <v>1</v>
       </c>
-      <c r="F18" s="24">
+      <c r="F18" s="23">
         <v>2</v>
       </c>
-      <c r="G18" s="24">
+      <c r="G18" s="23">
         <v>3</v>
       </c>
-      <c r="H18" s="24">
+      <c r="H18" s="23">
         <v>4</v>
       </c>
-      <c r="I18" s="24">
+      <c r="I18" s="23">
         <v>5</v>
       </c>
       <c r="J18" s="17">
@@ -1664,19 +1664,19 @@
       <c r="S18" s="17">
         <v>15</v>
       </c>
-      <c r="T18" s="24">
+      <c r="T18" s="23">
         <v>16</v>
       </c>
-      <c r="U18" s="24">
+      <c r="U18" s="23">
         <v>17</v>
       </c>
-      <c r="V18" s="24">
+      <c r="V18" s="23">
         <v>18</v>
       </c>
-      <c r="W18" s="25">
+      <c r="W18" s="24">
         <v>19</v>
       </c>
-      <c r="X18" s="24">
+      <c r="X18" s="23">
         <v>20</v>
       </c>
     </row>
@@ -1691,19 +1691,19 @@
         <f>AVERAGE(J19:S19)</f>
         <v>261</v>
       </c>
-      <c r="E19" s="19">
-        <v>261</v>
-      </c>
-      <c r="F19" s="19">
-        <v>261</v>
-      </c>
-      <c r="G19" s="19">
-        <v>261</v>
-      </c>
-      <c r="H19" s="19">
-        <v>261</v>
-      </c>
-      <c r="I19" s="19">
+      <c r="E19" s="18">
+        <v>261</v>
+      </c>
+      <c r="F19" s="18">
+        <v>261</v>
+      </c>
+      <c r="G19" s="18">
+        <v>261</v>
+      </c>
+      <c r="H19" s="18">
+        <v>261</v>
+      </c>
+      <c r="I19" s="18">
         <v>261</v>
       </c>
       <c r="J19" s="3">
@@ -1736,19 +1736,19 @@
       <c r="S19" s="3">
         <v>261</v>
       </c>
-      <c r="T19" s="19">
-        <v>261</v>
-      </c>
-      <c r="U19" s="19">
-        <v>261</v>
-      </c>
-      <c r="V19" s="19">
-        <v>261</v>
-      </c>
-      <c r="W19" s="19">
-        <v>261</v>
-      </c>
-      <c r="X19" s="19">
+      <c r="T19" s="18">
+        <v>261</v>
+      </c>
+      <c r="U19" s="18">
+        <v>261</v>
+      </c>
+      <c r="V19" s="18">
+        <v>261</v>
+      </c>
+      <c r="W19" s="18">
+        <v>261</v>
+      </c>
+      <c r="X19" s="18">
         <v>261</v>
       </c>
     </row>
@@ -1763,19 +1763,19 @@
         <f t="shared" ref="D20:D30" si="1">AVERAGE(J20:S20)</f>
         <v>477</v>
       </c>
-      <c r="E20" s="19">
-        <v>477</v>
-      </c>
-      <c r="F20" s="19">
-        <v>477</v>
-      </c>
-      <c r="G20" s="19">
-        <v>477</v>
-      </c>
-      <c r="H20" s="19">
-        <v>477</v>
-      </c>
-      <c r="I20" s="19">
+      <c r="E20" s="18">
+        <v>477</v>
+      </c>
+      <c r="F20" s="18">
+        <v>477</v>
+      </c>
+      <c r="G20" s="18">
+        <v>477</v>
+      </c>
+      <c r="H20" s="18">
+        <v>477</v>
+      </c>
+      <c r="I20" s="18">
         <v>477</v>
       </c>
       <c r="J20" s="3">
@@ -1808,19 +1808,19 @@
       <c r="S20" s="3">
         <v>477</v>
       </c>
-      <c r="T20" s="19">
-        <v>477</v>
-      </c>
-      <c r="U20" s="19">
-        <v>477</v>
-      </c>
-      <c r="V20" s="19">
-        <v>477</v>
-      </c>
-      <c r="W20" s="19">
-        <v>477</v>
-      </c>
-      <c r="X20" s="19">
+      <c r="T20" s="18">
+        <v>477</v>
+      </c>
+      <c r="U20" s="18">
+        <v>477</v>
+      </c>
+      <c r="V20" s="18">
+        <v>477</v>
+      </c>
+      <c r="W20" s="18">
+        <v>477</v>
+      </c>
+      <c r="X20" s="18">
         <v>477</v>
       </c>
     </row>
@@ -1835,19 +1835,19 @@
         <f t="shared" si="1"/>
         <v>1331</v>
       </c>
-      <c r="E21" s="19">
-        <v>1331</v>
-      </c>
-      <c r="F21" s="19">
-        <v>1331</v>
-      </c>
-      <c r="G21" s="19">
-        <v>1331</v>
-      </c>
-      <c r="H21" s="19">
-        <v>1331</v>
-      </c>
-      <c r="I21" s="19">
+      <c r="E21" s="18">
+        <v>1331</v>
+      </c>
+      <c r="F21" s="18">
+        <v>1331</v>
+      </c>
+      <c r="G21" s="18">
+        <v>1331</v>
+      </c>
+      <c r="H21" s="18">
+        <v>1331</v>
+      </c>
+      <c r="I21" s="18">
         <v>1331</v>
       </c>
       <c r="J21" s="3">
@@ -1880,19 +1880,19 @@
       <c r="S21" s="3">
         <v>1331</v>
       </c>
-      <c r="T21" s="19">
-        <v>1331</v>
-      </c>
-      <c r="U21" s="19">
-        <v>1331</v>
-      </c>
-      <c r="V21" s="19">
-        <v>1331</v>
-      </c>
-      <c r="W21" s="19">
-        <v>1331</v>
-      </c>
-      <c r="X21" s="19">
+      <c r="T21" s="18">
+        <v>1331</v>
+      </c>
+      <c r="U21" s="18">
+        <v>1331</v>
+      </c>
+      <c r="V21" s="18">
+        <v>1331</v>
+      </c>
+      <c r="W21" s="18">
+        <v>1331</v>
+      </c>
+      <c r="X21" s="18">
         <v>1331</v>
       </c>
     </row>
@@ -1907,19 +1907,19 @@
         <f t="shared" si="1"/>
         <v>261</v>
       </c>
-      <c r="E22" s="26">
-        <v>261</v>
-      </c>
-      <c r="F22" s="26">
-        <v>261</v>
-      </c>
-      <c r="G22" s="26">
-        <v>261</v>
-      </c>
-      <c r="H22" s="26">
-        <v>261</v>
-      </c>
-      <c r="I22" s="26">
+      <c r="E22" s="25">
+        <v>261</v>
+      </c>
+      <c r="F22" s="25">
+        <v>261</v>
+      </c>
+      <c r="G22" s="25">
+        <v>261</v>
+      </c>
+      <c r="H22" s="25">
+        <v>261</v>
+      </c>
+      <c r="I22" s="25">
         <v>261</v>
       </c>
       <c r="J22" s="9">
@@ -1952,19 +1952,19 @@
       <c r="S22" s="9">
         <v>261</v>
       </c>
-      <c r="T22" s="26">
-        <v>261</v>
-      </c>
-      <c r="U22" s="26">
-        <v>261</v>
-      </c>
-      <c r="V22" s="26">
-        <v>261</v>
-      </c>
-      <c r="W22" s="26">
-        <v>261</v>
-      </c>
-      <c r="X22" s="26">
+      <c r="T22" s="25">
+        <v>261</v>
+      </c>
+      <c r="U22" s="25">
+        <v>261</v>
+      </c>
+      <c r="V22" s="25">
+        <v>261</v>
+      </c>
+      <c r="W22" s="25">
+        <v>261</v>
+      </c>
+      <c r="X22" s="25">
         <v>261</v>
       </c>
     </row>
@@ -1979,19 +1979,19 @@
         <f t="shared" si="1"/>
         <v>477</v>
       </c>
-      <c r="E23" s="26">
-        <v>477</v>
-      </c>
-      <c r="F23" s="26">
-        <v>477</v>
-      </c>
-      <c r="G23" s="26">
-        <v>477</v>
-      </c>
-      <c r="H23" s="26">
-        <v>477</v>
-      </c>
-      <c r="I23" s="26">
+      <c r="E23" s="25">
+        <v>477</v>
+      </c>
+      <c r="F23" s="25">
+        <v>477</v>
+      </c>
+      <c r="G23" s="25">
+        <v>477</v>
+      </c>
+      <c r="H23" s="25">
+        <v>477</v>
+      </c>
+      <c r="I23" s="25">
         <v>477</v>
       </c>
       <c r="J23" s="9">
@@ -2024,19 +2024,19 @@
       <c r="S23" s="9">
         <v>477</v>
       </c>
-      <c r="T23" s="26">
-        <v>477</v>
-      </c>
-      <c r="U23" s="26">
-        <v>477</v>
-      </c>
-      <c r="V23" s="26">
-        <v>477</v>
-      </c>
-      <c r="W23" s="26">
-        <v>477</v>
-      </c>
-      <c r="X23" s="26">
+      <c r="T23" s="25">
+        <v>477</v>
+      </c>
+      <c r="U23" s="25">
+        <v>477</v>
+      </c>
+      <c r="V23" s="25">
+        <v>477</v>
+      </c>
+      <c r="W23" s="25">
+        <v>477</v>
+      </c>
+      <c r="X23" s="25">
         <v>477</v>
       </c>
     </row>
@@ -2051,19 +2051,19 @@
         <f t="shared" si="1"/>
         <v>1331</v>
       </c>
-      <c r="E24" s="26">
-        <v>1331</v>
-      </c>
-      <c r="F24" s="26">
-        <v>1331</v>
-      </c>
-      <c r="G24" s="26">
-        <v>1331</v>
-      </c>
-      <c r="H24" s="26">
-        <v>1331</v>
-      </c>
-      <c r="I24" s="26">
+      <c r="E24" s="25">
+        <v>1331</v>
+      </c>
+      <c r="F24" s="25">
+        <v>1331</v>
+      </c>
+      <c r="G24" s="25">
+        <v>1331</v>
+      </c>
+      <c r="H24" s="25">
+        <v>1331</v>
+      </c>
+      <c r="I24" s="25">
         <v>1331</v>
       </c>
       <c r="J24" s="9">
@@ -2096,19 +2096,19 @@
       <c r="S24" s="9">
         <v>1331</v>
       </c>
-      <c r="T24" s="26">
-        <v>1331</v>
-      </c>
-      <c r="U24" s="26">
-        <v>1331</v>
-      </c>
-      <c r="V24" s="26">
-        <v>1331</v>
-      </c>
-      <c r="W24" s="26">
-        <v>1331</v>
-      </c>
-      <c r="X24" s="26">
+      <c r="T24" s="25">
+        <v>1331</v>
+      </c>
+      <c r="U24" s="25">
+        <v>1331</v>
+      </c>
+      <c r="V24" s="25">
+        <v>1331</v>
+      </c>
+      <c r="W24" s="25">
+        <v>1331</v>
+      </c>
+      <c r="X24" s="25">
         <v>1331</v>
       </c>
     </row>
@@ -2123,19 +2123,19 @@
         <f t="shared" si="1"/>
         <v>261</v>
       </c>
-      <c r="E25" s="19">
-        <v>261</v>
-      </c>
-      <c r="F25" s="19">
-        <v>261</v>
-      </c>
-      <c r="G25" s="19">
-        <v>261</v>
-      </c>
-      <c r="H25" s="19">
-        <v>261</v>
-      </c>
-      <c r="I25" s="19">
+      <c r="E25" s="18">
+        <v>261</v>
+      </c>
+      <c r="F25" s="18">
+        <v>261</v>
+      </c>
+      <c r="G25" s="18">
+        <v>261</v>
+      </c>
+      <c r="H25" s="18">
+        <v>261</v>
+      </c>
+      <c r="I25" s="18">
         <v>261</v>
       </c>
       <c r="J25" s="3">
@@ -2168,19 +2168,19 @@
       <c r="S25" s="3">
         <v>261</v>
       </c>
-      <c r="T25" s="19">
-        <v>261</v>
-      </c>
-      <c r="U25" s="19">
-        <v>261</v>
-      </c>
-      <c r="V25" s="19">
-        <v>261</v>
-      </c>
-      <c r="W25" s="19">
-        <v>261</v>
-      </c>
-      <c r="X25" s="19">
+      <c r="T25" s="18">
+        <v>261</v>
+      </c>
+      <c r="U25" s="18">
+        <v>261</v>
+      </c>
+      <c r="V25" s="18">
+        <v>261</v>
+      </c>
+      <c r="W25" s="18">
+        <v>261</v>
+      </c>
+      <c r="X25" s="18">
         <v>261</v>
       </c>
     </row>
@@ -2195,19 +2195,19 @@
         <f t="shared" si="1"/>
         <v>477</v>
       </c>
-      <c r="E26" s="19">
-        <v>477</v>
-      </c>
-      <c r="F26" s="19">
-        <v>477</v>
-      </c>
-      <c r="G26" s="19">
-        <v>477</v>
-      </c>
-      <c r="H26" s="19">
-        <v>477</v>
-      </c>
-      <c r="I26" s="19">
+      <c r="E26" s="18">
+        <v>477</v>
+      </c>
+      <c r="F26" s="18">
+        <v>477</v>
+      </c>
+      <c r="G26" s="18">
+        <v>477</v>
+      </c>
+      <c r="H26" s="18">
+        <v>477</v>
+      </c>
+      <c r="I26" s="18">
         <v>477</v>
       </c>
       <c r="J26" s="3">
@@ -2240,19 +2240,19 @@
       <c r="S26" s="3">
         <v>477</v>
       </c>
-      <c r="T26" s="19">
-        <v>477</v>
-      </c>
-      <c r="U26" s="19">
-        <v>477</v>
-      </c>
-      <c r="V26" s="19">
-        <v>477</v>
-      </c>
-      <c r="W26" s="19">
-        <v>477</v>
-      </c>
-      <c r="X26" s="19">
+      <c r="T26" s="18">
+        <v>477</v>
+      </c>
+      <c r="U26" s="18">
+        <v>477</v>
+      </c>
+      <c r="V26" s="18">
+        <v>477</v>
+      </c>
+      <c r="W26" s="18">
+        <v>477</v>
+      </c>
+      <c r="X26" s="18">
         <v>477</v>
       </c>
     </row>
@@ -2267,19 +2267,19 @@
         <f t="shared" si="1"/>
         <v>1331</v>
       </c>
-      <c r="E27" s="19">
-        <v>1331</v>
-      </c>
-      <c r="F27" s="19">
-        <v>1331</v>
-      </c>
-      <c r="G27" s="19">
-        <v>1331</v>
-      </c>
-      <c r="H27" s="19">
-        <v>1331</v>
-      </c>
-      <c r="I27" s="19">
+      <c r="E27" s="18">
+        <v>1331</v>
+      </c>
+      <c r="F27" s="18">
+        <v>1331</v>
+      </c>
+      <c r="G27" s="18">
+        <v>1331</v>
+      </c>
+      <c r="H27" s="18">
+        <v>1331</v>
+      </c>
+      <c r="I27" s="18">
         <v>1331</v>
       </c>
       <c r="J27" s="3">
@@ -2312,19 +2312,19 @@
       <c r="S27" s="3">
         <v>1331</v>
       </c>
-      <c r="T27" s="19">
-        <v>1331</v>
-      </c>
-      <c r="U27" s="19">
-        <v>1331</v>
-      </c>
-      <c r="V27" s="19">
-        <v>1331</v>
-      </c>
-      <c r="W27" s="19">
-        <v>1331</v>
-      </c>
-      <c r="X27" s="19">
+      <c r="T27" s="18">
+        <v>1331</v>
+      </c>
+      <c r="U27" s="18">
+        <v>1331</v>
+      </c>
+      <c r="V27" s="18">
+        <v>1331</v>
+      </c>
+      <c r="W27" s="18">
+        <v>1331</v>
+      </c>
+      <c r="X27" s="18">
         <v>1331</v>
       </c>
     </row>
@@ -2339,19 +2339,19 @@
         <f t="shared" si="1"/>
         <v>261</v>
       </c>
-      <c r="E28" s="26">
-        <v>261</v>
-      </c>
-      <c r="F28" s="26">
-        <v>261</v>
-      </c>
-      <c r="G28" s="26">
-        <v>261</v>
-      </c>
-      <c r="H28" s="26">
-        <v>261</v>
-      </c>
-      <c r="I28" s="26">
+      <c r="E28" s="25">
+        <v>261</v>
+      </c>
+      <c r="F28" s="25">
+        <v>261</v>
+      </c>
+      <c r="G28" s="25">
+        <v>261</v>
+      </c>
+      <c r="H28" s="25">
+        <v>261</v>
+      </c>
+      <c r="I28" s="25">
         <v>261</v>
       </c>
       <c r="J28" s="9">
@@ -2384,19 +2384,19 @@
       <c r="S28" s="9">
         <v>261</v>
       </c>
-      <c r="T28" s="26">
-        <v>261</v>
-      </c>
-      <c r="U28" s="26">
-        <v>261</v>
-      </c>
-      <c r="V28" s="26">
-        <v>261</v>
-      </c>
-      <c r="W28" s="26">
-        <v>261</v>
-      </c>
-      <c r="X28" s="26">
+      <c r="T28" s="25">
+        <v>261</v>
+      </c>
+      <c r="U28" s="25">
+        <v>261</v>
+      </c>
+      <c r="V28" s="25">
+        <v>261</v>
+      </c>
+      <c r="W28" s="25">
+        <v>261</v>
+      </c>
+      <c r="X28" s="25">
         <v>261</v>
       </c>
     </row>
@@ -2411,19 +2411,19 @@
         <f t="shared" si="1"/>
         <v>477</v>
       </c>
-      <c r="E29" s="26">
-        <v>477</v>
-      </c>
-      <c r="F29" s="26">
-        <v>477</v>
-      </c>
-      <c r="G29" s="26">
-        <v>477</v>
-      </c>
-      <c r="H29" s="26">
-        <v>477</v>
-      </c>
-      <c r="I29" s="26">
+      <c r="E29" s="25">
+        <v>477</v>
+      </c>
+      <c r="F29" s="25">
+        <v>477</v>
+      </c>
+      <c r="G29" s="25">
+        <v>477</v>
+      </c>
+      <c r="H29" s="25">
+        <v>477</v>
+      </c>
+      <c r="I29" s="25">
         <v>477</v>
       </c>
       <c r="J29" s="9">
@@ -2456,19 +2456,19 @@
       <c r="S29" s="9">
         <v>477</v>
       </c>
-      <c r="T29" s="26">
-        <v>477</v>
-      </c>
-      <c r="U29" s="26">
-        <v>477</v>
-      </c>
-      <c r="V29" s="26">
-        <v>477</v>
-      </c>
-      <c r="W29" s="26">
-        <v>477</v>
-      </c>
-      <c r="X29" s="26">
+      <c r="T29" s="25">
+        <v>477</v>
+      </c>
+      <c r="U29" s="25">
+        <v>477</v>
+      </c>
+      <c r="V29" s="25">
+        <v>477</v>
+      </c>
+      <c r="W29" s="25">
+        <v>477</v>
+      </c>
+      <c r="X29" s="25">
         <v>477</v>
       </c>
     </row>
@@ -2483,19 +2483,19 @@
         <f t="shared" si="1"/>
         <v>1331</v>
       </c>
-      <c r="E30" s="26">
-        <v>1331</v>
-      </c>
-      <c r="F30" s="26">
-        <v>1331</v>
-      </c>
-      <c r="G30" s="26">
-        <v>1331</v>
-      </c>
-      <c r="H30" s="26">
-        <v>1331</v>
-      </c>
-      <c r="I30" s="26">
+      <c r="E30" s="25">
+        <v>1331</v>
+      </c>
+      <c r="F30" s="25">
+        <v>1331</v>
+      </c>
+      <c r="G30" s="25">
+        <v>1331</v>
+      </c>
+      <c r="H30" s="25">
+        <v>1331</v>
+      </c>
+      <c r="I30" s="25">
         <v>1331</v>
       </c>
       <c r="J30" s="9">
@@ -2528,19 +2528,19 @@
       <c r="S30" s="9">
         <v>1331</v>
       </c>
-      <c r="T30" s="26">
-        <v>1331</v>
-      </c>
-      <c r="U30" s="26">
-        <v>1331</v>
-      </c>
-      <c r="V30" s="26">
-        <v>1331</v>
-      </c>
-      <c r="W30" s="26">
-        <v>1331</v>
-      </c>
-      <c r="X30" s="26">
+      <c r="T30" s="25">
+        <v>1331</v>
+      </c>
+      <c r="U30" s="25">
+        <v>1331</v>
+      </c>
+      <c r="V30" s="25">
+        <v>1331</v>
+      </c>
+      <c r="W30" s="25">
+        <v>1331</v>
+      </c>
+      <c r="X30" s="25">
         <v>1331</v>
       </c>
     </row>
@@ -2556,8 +2556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051415FD-3633-4903-A550-646AFA39BC19}">
   <dimension ref="B2:X30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2583,19 +2583,19 @@
       <c r="D3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="23">
         <v>1</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="23">
         <v>2</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="23">
         <v>3</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="23">
         <v>4</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="23">
         <v>5</v>
       </c>
       <c r="J3" s="17">
@@ -2628,19 +2628,19 @@
       <c r="S3" s="17">
         <v>15</v>
       </c>
-      <c r="T3" s="17">
+      <c r="T3" s="23">
         <v>16</v>
       </c>
-      <c r="U3" s="17">
+      <c r="U3" s="23">
         <v>17</v>
       </c>
-      <c r="V3" s="17">
+      <c r="V3" s="23">
         <v>18</v>
       </c>
-      <c r="W3" s="16">
+      <c r="W3" s="24">
         <v>19</v>
       </c>
-      <c r="X3" s="17">
+      <c r="X3" s="23">
         <v>20</v>
       </c>
     </row>
@@ -2652,68 +2652,68 @@
         <v>1</v>
       </c>
       <c r="D4" s="3">
-        <f>AVERAGE(E4:AC4)</f>
-        <v>517.15</v>
-      </c>
-      <c r="E4" s="3">
-        <v>518</v>
-      </c>
-      <c r="F4" s="3">
-        <v>517</v>
-      </c>
-      <c r="G4" s="3">
-        <v>544</v>
-      </c>
-      <c r="H4" s="3">
-        <v>514</v>
-      </c>
-      <c r="I4" s="3">
-        <v>515</v>
+        <f>AVERAGE(J4:S4)</f>
+        <v>514.20000000000005</v>
+      </c>
+      <c r="E4" s="18">
+        <v>511</v>
+      </c>
+      <c r="F4" s="18">
+        <v>512</v>
+      </c>
+      <c r="G4" s="18">
+        <v>512</v>
+      </c>
+      <c r="H4" s="18">
+        <v>513</v>
+      </c>
+      <c r="I4" s="18">
+        <v>513</v>
       </c>
       <c r="J4" s="3">
         <v>513</v>
       </c>
       <c r="K4" s="3">
+        <v>513</v>
+      </c>
+      <c r="L4" s="3">
         <v>514</v>
       </c>
-      <c r="L4" s="3">
-        <v>545</v>
-      </c>
       <c r="M4" s="3">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="N4" s="3">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="O4" s="3">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="P4" s="3">
         <v>515</v>
       </c>
       <c r="Q4" s="3">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="R4" s="3">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="S4" s="3">
+        <v>515</v>
+      </c>
+      <c r="T4" s="18">
         <v>516</v>
       </c>
-      <c r="T4" s="3">
-        <v>515</v>
-      </c>
-      <c r="U4" s="3">
-        <v>511</v>
-      </c>
-      <c r="V4" s="3">
-        <v>514</v>
-      </c>
-      <c r="W4" s="2">
-        <v>514</v>
-      </c>
-      <c r="X4" s="18">
-        <v>512</v>
+      <c r="U4" s="18">
+        <v>517</v>
+      </c>
+      <c r="V4" s="18">
+        <v>518</v>
+      </c>
+      <c r="W4" s="21">
+        <v>544</v>
+      </c>
+      <c r="X4" s="28">
+        <v>545</v>
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.3">
@@ -2724,68 +2724,68 @@
         <v>2</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D15" si="0">AVERAGE(E5:AC5)</f>
-        <v>686.9</v>
-      </c>
-      <c r="E5" s="6">
-        <v>688</v>
-      </c>
-      <c r="F5" s="6">
-        <v>695</v>
-      </c>
-      <c r="G5" s="6">
-        <v>688</v>
-      </c>
-      <c r="H5" s="6">
+        <f t="shared" ref="D5:D15" si="0">AVERAGE(J5:S5)</f>
+        <v>686.8</v>
+      </c>
+      <c r="E5" s="19">
+        <v>682</v>
+      </c>
+      <c r="F5" s="19">
         <v>684</v>
       </c>
-      <c r="I5" s="6">
+      <c r="G5" s="19">
+        <v>684</v>
+      </c>
+      <c r="H5" s="19">
+        <v>685</v>
+      </c>
+      <c r="I5" s="19">
         <v>685</v>
       </c>
       <c r="J5" s="6">
         <v>685</v>
       </c>
       <c r="K5" s="6">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="L5" s="6">
+        <v>686</v>
+      </c>
+      <c r="M5" s="6">
+        <v>687</v>
+      </c>
+      <c r="N5" s="6">
+        <v>687</v>
+      </c>
+      <c r="O5" s="6">
+        <v>687</v>
+      </c>
+      <c r="P5" s="6">
+        <v>687</v>
+      </c>
+      <c r="Q5" s="6">
         <v>688</v>
       </c>
-      <c r="M5" s="6">
-        <v>685</v>
-      </c>
-      <c r="N5" s="6">
-        <v>682</v>
-      </c>
-      <c r="O5" s="6">
+      <c r="R5" s="6">
+        <v>688</v>
+      </c>
+      <c r="S5" s="6">
+        <v>688</v>
+      </c>
+      <c r="T5" s="19">
+        <v>688</v>
+      </c>
+      <c r="U5" s="19">
+        <v>688</v>
+      </c>
+      <c r="V5" s="19">
+        <v>689</v>
+      </c>
+      <c r="W5" s="22">
         <v>690</v>
       </c>
-      <c r="P5" s="6">
-        <v>689</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>686</v>
-      </c>
-      <c r="R5" s="6">
-        <v>685</v>
-      </c>
-      <c r="S5" s="6">
-        <v>687</v>
-      </c>
-      <c r="T5" s="6">
-        <v>687</v>
-      </c>
-      <c r="U5" s="6">
-        <v>688</v>
-      </c>
-      <c r="V5" s="6">
-        <v>688</v>
-      </c>
-      <c r="W5" s="5">
-        <v>687</v>
-      </c>
-      <c r="X5" s="6">
-        <v>687</v>
+      <c r="X5" s="19">
+        <v>695</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
@@ -2797,67 +2797,67 @@
       </c>
       <c r="D6" s="3">
         <f t="shared" si="0"/>
-        <v>1301.5</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1313</v>
-      </c>
-      <c r="F6" s="6">
+        <v>1304.2</v>
+      </c>
+      <c r="E6" s="19">
+        <v>1286</v>
+      </c>
+      <c r="F6" s="19">
+        <v>1288</v>
+      </c>
+      <c r="G6" s="19">
+        <v>1288</v>
+      </c>
+      <c r="H6" s="19">
         <v>1289</v>
       </c>
-      <c r="G6" s="6">
-        <v>1309</v>
-      </c>
-      <c r="H6" s="6">
+      <c r="I6" s="19">
+        <v>1289</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1290</v>
+      </c>
+      <c r="K6" s="6">
+        <v>1303</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1304</v>
+      </c>
+      <c r="M6" s="6">
         <v>1306</v>
       </c>
-      <c r="I6" s="6">
-        <v>1288</v>
-      </c>
-      <c r="J6" s="6">
-        <v>1308</v>
-      </c>
-      <c r="K6" s="6">
-        <v>1309</v>
-      </c>
-      <c r="L6" s="6">
-        <v>1289</v>
-      </c>
-      <c r="M6" s="6">
-        <v>1307</v>
-      </c>
       <c r="N6" s="6">
-        <v>1303</v>
+        <v>1306</v>
       </c>
       <c r="O6" s="6">
         <v>1306</v>
       </c>
       <c r="P6" s="6">
+        <v>1306</v>
+      </c>
+      <c r="Q6" s="6">
         <v>1307</v>
       </c>
-      <c r="Q6" s="6">
-        <v>1290</v>
-      </c>
       <c r="R6" s="6">
-        <v>1304</v>
+        <v>1307</v>
       </c>
       <c r="S6" s="6">
+        <v>1307</v>
+      </c>
+      <c r="T6" s="19">
+        <v>1308</v>
+      </c>
+      <c r="U6" s="19">
         <v>1309</v>
       </c>
-      <c r="T6" s="6">
-        <v>1306</v>
-      </c>
-      <c r="U6" s="6">
-        <v>1286</v>
-      </c>
-      <c r="V6" s="6">
-        <v>1306</v>
-      </c>
-      <c r="W6" s="5">
-        <v>1307</v>
-      </c>
-      <c r="X6" s="6">
-        <v>1288</v>
+      <c r="V6" s="19">
+        <v>1309</v>
+      </c>
+      <c r="W6" s="22">
+        <v>1309</v>
+      </c>
+      <c r="X6" s="19">
+        <v>1313</v>
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
@@ -2869,67 +2869,67 @@
       </c>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
-        <v>515.15</v>
-      </c>
-      <c r="E7" s="10">
-        <v>532</v>
-      </c>
-      <c r="F7" s="10">
-        <v>515</v>
-      </c>
-      <c r="G7" s="10">
+        <v>514.29999999999995</v>
+      </c>
+      <c r="E7" s="26">
+        <v>512</v>
+      </c>
+      <c r="F7" s="26">
+        <v>512</v>
+      </c>
+      <c r="G7" s="26">
+        <v>512</v>
+      </c>
+      <c r="H7" s="26">
         <v>513</v>
       </c>
-      <c r="H7" s="10">
-        <v>512</v>
-      </c>
-      <c r="I7" s="10">
-        <v>516</v>
+      <c r="I7" s="26">
+        <v>513</v>
       </c>
       <c r="J7" s="10">
         <v>513</v>
       </c>
       <c r="K7" s="10">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="L7" s="10">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="M7" s="10">
         <v>513</v>
       </c>
       <c r="N7" s="10">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="O7" s="10">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="P7" s="10">
         <v>515</v>
       </c>
       <c r="Q7" s="10">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="R7" s="10">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="S7" s="10">
         <v>516</v>
       </c>
-      <c r="T7" s="10">
-        <v>513</v>
-      </c>
-      <c r="U7" s="10">
-        <v>513</v>
-      </c>
-      <c r="V7" s="10">
+      <c r="T7" s="26">
         <v>516</v>
       </c>
-      <c r="W7" s="8">
-        <v>513</v>
-      </c>
-      <c r="X7" s="10">
+      <c r="U7" s="26">
         <v>516</v>
+      </c>
+      <c r="V7" s="26">
+        <v>517</v>
+      </c>
+      <c r="W7" s="27">
+        <v>517</v>
+      </c>
+      <c r="X7" s="26">
+        <v>532</v>
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
@@ -2941,67 +2941,67 @@
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
-        <v>694.05</v>
-      </c>
-      <c r="E8" s="10">
-        <v>711</v>
-      </c>
-      <c r="F8" s="10">
-        <v>688</v>
-      </c>
-      <c r="G8" s="10">
+        <v>692</v>
+      </c>
+      <c r="E8" s="26">
+        <v>683</v>
+      </c>
+      <c r="F8" s="26">
+        <v>684</v>
+      </c>
+      <c r="G8" s="26">
         <v>686</v>
       </c>
-      <c r="H8" s="10">
-        <v>699</v>
-      </c>
-      <c r="I8" s="10">
+      <c r="H8" s="26">
         <v>686</v>
       </c>
+      <c r="I8" s="26">
+        <v>686</v>
+      </c>
       <c r="J8" s="10">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="K8" s="10">
-        <v>708</v>
+        <v>687</v>
       </c>
       <c r="L8" s="10">
         <v>687</v>
       </c>
       <c r="M8" s="10">
+        <v>687</v>
+      </c>
+      <c r="N8" s="10">
+        <v>688</v>
+      </c>
+      <c r="O8" s="10">
+        <v>689</v>
+      </c>
+      <c r="P8" s="10">
+        <v>690</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>699</v>
+      </c>
+      <c r="R8" s="10">
+        <v>703</v>
+      </c>
+      <c r="S8" s="10">
+        <v>703</v>
+      </c>
+      <c r="T8" s="26">
         <v>704</v>
       </c>
-      <c r="N8" s="10">
+      <c r="U8" s="26">
+        <v>706</v>
+      </c>
+      <c r="V8" s="26">
         <v>707</v>
       </c>
-      <c r="O8" s="10">
-        <v>686</v>
-      </c>
-      <c r="P8" s="10">
-        <v>703</v>
-      </c>
-      <c r="Q8" s="10">
-        <v>687</v>
-      </c>
-      <c r="R8" s="10">
-        <v>687</v>
-      </c>
-      <c r="S8" s="10">
-        <v>687</v>
-      </c>
-      <c r="T8" s="10">
-        <v>684</v>
-      </c>
-      <c r="U8" s="10">
-        <v>703</v>
-      </c>
-      <c r="V8" s="10">
-        <v>689</v>
-      </c>
-      <c r="W8" s="8">
-        <v>706</v>
-      </c>
-      <c r="X8" s="10">
-        <v>690</v>
+      <c r="W8" s="27">
+        <v>708</v>
+      </c>
+      <c r="X8" s="26">
+        <v>711</v>
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
@@ -3013,67 +3013,67 @@
       </c>
       <c r="D9" s="9">
         <f t="shared" si="0"/>
-        <v>1298.6500000000001</v>
-      </c>
-      <c r="E9" s="10">
+        <v>1299</v>
+      </c>
+      <c r="E9" s="26">
+        <v>1286</v>
+      </c>
+      <c r="F9" s="26">
+        <v>1287</v>
+      </c>
+      <c r="G9" s="26">
+        <v>1288</v>
+      </c>
+      <c r="H9" s="26">
+        <v>1289</v>
+      </c>
+      <c r="I9" s="26">
+        <v>1290</v>
+      </c>
+      <c r="J9" s="10">
+        <v>1290</v>
+      </c>
+      <c r="K9" s="10">
+        <v>1290</v>
+      </c>
+      <c r="L9" s="10">
+        <v>1290</v>
+      </c>
+      <c r="M9" s="10">
+        <v>1292</v>
+      </c>
+      <c r="N9" s="10">
+        <v>1304</v>
+      </c>
+      <c r="O9" s="10">
+        <v>1304</v>
+      </c>
+      <c r="P9" s="10">
         <v>1305</v>
       </c>
-      <c r="F9" s="10">
-        <v>1290</v>
-      </c>
-      <c r="G9" s="10">
+      <c r="Q9" s="10">
+        <v>1305</v>
+      </c>
+      <c r="R9" s="10">
+        <v>1305</v>
+      </c>
+      <c r="S9" s="10">
+        <v>1305</v>
+      </c>
+      <c r="T9" s="26">
+        <v>1306</v>
+      </c>
+      <c r="U9" s="26">
+        <v>1306</v>
+      </c>
+      <c r="V9" s="26">
+        <v>1307</v>
+      </c>
+      <c r="W9" s="27">
         <v>1308</v>
       </c>
-      <c r="H9" s="10">
-        <v>1305</v>
-      </c>
-      <c r="I9" s="10">
-        <v>1286</v>
-      </c>
-      <c r="J9" s="10">
-        <v>1287</v>
-      </c>
-      <c r="K9" s="10">
-        <v>1306</v>
-      </c>
-      <c r="L9" s="10">
-        <v>1288</v>
-      </c>
-      <c r="M9" s="10">
-        <v>1305</v>
-      </c>
-      <c r="N9" s="10">
-        <v>1307</v>
-      </c>
-      <c r="O9" s="10">
+      <c r="X9" s="26">
         <v>1316</v>
-      </c>
-      <c r="P9" s="10">
-        <v>1304</v>
-      </c>
-      <c r="Q9" s="10">
-        <v>1290</v>
-      </c>
-      <c r="R9" s="10">
-        <v>1290</v>
-      </c>
-      <c r="S9" s="10">
-        <v>1290</v>
-      </c>
-      <c r="T9" s="10">
-        <v>1304</v>
-      </c>
-      <c r="U9" s="10">
-        <v>1305</v>
-      </c>
-      <c r="V9" s="10">
-        <v>1289</v>
-      </c>
-      <c r="W9" s="8">
-        <v>1306</v>
-      </c>
-      <c r="X9" s="10">
-        <v>1292</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
@@ -3085,67 +3085,67 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" si="0"/>
-        <v>524.75</v>
-      </c>
-      <c r="E10" s="6">
-        <v>537</v>
-      </c>
-      <c r="F10" s="6">
-        <v>536</v>
-      </c>
-      <c r="G10" s="6">
-        <v>534</v>
-      </c>
-      <c r="H10" s="6">
+        <v>524.6</v>
+      </c>
+      <c r="E10" s="19">
+        <v>512</v>
+      </c>
+      <c r="F10" s="19">
         <v>513</v>
       </c>
-      <c r="I10" s="6">
-        <v>519</v>
+      <c r="G10" s="19">
+        <v>513</v>
+      </c>
+      <c r="H10" s="19">
+        <v>514</v>
+      </c>
+      <c r="I10" s="19">
+        <v>516</v>
       </c>
       <c r="J10" s="6">
-        <v>532</v>
+        <v>516</v>
       </c>
       <c r="K10" s="6">
-        <v>537</v>
+        <v>517</v>
       </c>
       <c r="L10" s="6">
-        <v>531</v>
+        <v>517</v>
       </c>
       <c r="M10" s="6">
         <v>518</v>
       </c>
       <c r="N10" s="6">
+        <v>519</v>
+      </c>
+      <c r="O10" s="6">
+        <v>530</v>
+      </c>
+      <c r="P10" s="6">
+        <v>531</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>532</v>
+      </c>
+      <c r="R10" s="6">
+        <v>532</v>
+      </c>
+      <c r="S10" s="6">
+        <v>534</v>
+      </c>
+      <c r="T10" s="19">
+        <v>534</v>
+      </c>
+      <c r="U10" s="19">
+        <v>536</v>
+      </c>
+      <c r="V10" s="19">
         <v>537</v>
       </c>
-      <c r="O10" s="6">
-        <v>512</v>
-      </c>
-      <c r="P10" s="6">
-        <v>517</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>517</v>
-      </c>
-      <c r="R10" s="6">
-        <v>534</v>
-      </c>
-      <c r="S10" s="6">
-        <v>514</v>
-      </c>
-      <c r="T10" s="6">
-        <v>513</v>
-      </c>
-      <c r="U10" s="6">
-        <v>530</v>
-      </c>
-      <c r="V10" s="6">
-        <v>516</v>
-      </c>
-      <c r="W10" s="5">
-        <v>516</v>
-      </c>
-      <c r="X10" s="6">
-        <v>532</v>
+      <c r="W10" s="22">
+        <v>537</v>
+      </c>
+      <c r="X10" s="19">
+        <v>537</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.3">
@@ -3157,67 +3157,67 @@
       </c>
       <c r="D11" s="3">
         <f t="shared" si="0"/>
-        <v>696.25</v>
-      </c>
-      <c r="E11" s="6">
-        <v>712</v>
-      </c>
-      <c r="F11" s="6">
-        <v>704</v>
-      </c>
-      <c r="G11" s="6">
-        <v>707</v>
-      </c>
-      <c r="H11" s="6">
+        <v>696.2</v>
+      </c>
+      <c r="E11" s="19">
         <v>684</v>
       </c>
-      <c r="I11" s="6">
-        <v>690</v>
+      <c r="F11" s="19">
+        <v>685</v>
+      </c>
+      <c r="G11" s="19">
+        <v>685</v>
+      </c>
+      <c r="H11" s="19">
+        <v>686</v>
+      </c>
+      <c r="I11" s="19">
+        <v>686</v>
       </c>
       <c r="J11" s="6">
-        <v>704</v>
+        <v>687</v>
       </c>
       <c r="K11" s="6">
-        <v>707</v>
+        <v>688</v>
       </c>
       <c r="L11" s="6">
-        <v>704</v>
+        <v>689</v>
       </c>
       <c r="M11" s="6">
         <v>689</v>
       </c>
       <c r="N11" s="6">
+        <v>690</v>
+      </c>
+      <c r="O11" s="6">
+        <v>703</v>
+      </c>
+      <c r="P11" s="6">
+        <v>704</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>704</v>
+      </c>
+      <c r="R11" s="6">
+        <v>704</v>
+      </c>
+      <c r="S11" s="6">
+        <v>704</v>
+      </c>
+      <c r="T11" s="19">
+        <v>705</v>
+      </c>
+      <c r="U11" s="19">
         <v>706</v>
       </c>
-      <c r="O11" s="6">
-        <v>685</v>
-      </c>
-      <c r="P11" s="6">
-        <v>688</v>
-      </c>
-      <c r="Q11" s="6">
-        <v>685</v>
-      </c>
-      <c r="R11" s="6">
-        <v>705</v>
-      </c>
-      <c r="S11" s="6">
-        <v>686</v>
-      </c>
-      <c r="T11" s="6">
-        <v>686</v>
-      </c>
-      <c r="U11" s="6">
-        <v>704</v>
-      </c>
-      <c r="V11" s="6">
-        <v>689</v>
-      </c>
-      <c r="W11" s="5">
-        <v>687</v>
-      </c>
-      <c r="X11" s="6">
-        <v>703</v>
+      <c r="V11" s="19">
+        <v>707</v>
+      </c>
+      <c r="W11" s="22">
+        <v>707</v>
+      </c>
+      <c r="X11" s="19">
+        <v>712</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">
@@ -3231,65 +3231,65 @@
         <f t="shared" si="0"/>
         <v>1297.5</v>
       </c>
-      <c r="E12" s="6">
-        <v>1312</v>
-      </c>
-      <c r="F12" s="6">
-        <v>1307</v>
-      </c>
-      <c r="G12" s="6">
-        <v>1307</v>
-      </c>
-      <c r="H12" s="6">
+      <c r="E12" s="19">
         <v>1286</v>
       </c>
-      <c r="I12" s="6">
+      <c r="F12" s="19">
+        <v>1286</v>
+      </c>
+      <c r="G12" s="19">
+        <v>1287</v>
+      </c>
+      <c r="H12" s="19">
         <v>1288</v>
       </c>
+      <c r="I12" s="19">
+        <v>1288</v>
+      </c>
       <c r="J12" s="6">
-        <v>1305</v>
+        <v>1288</v>
       </c>
       <c r="K12" s="6">
-        <v>1307</v>
+        <v>1289</v>
       </c>
       <c r="L12" s="6">
-        <v>1305</v>
+        <v>1289</v>
       </c>
       <c r="M12" s="6">
         <v>1290</v>
       </c>
       <c r="N12" s="6">
-        <v>1307</v>
+        <v>1290</v>
       </c>
       <c r="O12" s="6">
-        <v>1288</v>
+        <v>1305</v>
       </c>
       <c r="P12" s="6">
-        <v>1290</v>
+        <v>1305</v>
       </c>
       <c r="Q12" s="6">
-        <v>1286</v>
+        <v>1305</v>
       </c>
       <c r="R12" s="6">
         <v>1307</v>
       </c>
       <c r="S12" s="6">
-        <v>1289</v>
-      </c>
-      <c r="T12" s="6">
-        <v>1289</v>
-      </c>
-      <c r="U12" s="6">
-        <v>1305</v>
-      </c>
-      <c r="V12" s="6">
-        <v>1287</v>
-      </c>
-      <c r="W12" s="5">
-        <v>1288</v>
-      </c>
-      <c r="X12" s="6">
         <v>1307</v>
+      </c>
+      <c r="T12" s="19">
+        <v>1307</v>
+      </c>
+      <c r="U12" s="19">
+        <v>1307</v>
+      </c>
+      <c r="V12" s="19">
+        <v>1307</v>
+      </c>
+      <c r="W12" s="22">
+        <v>1307</v>
+      </c>
+      <c r="X12" s="19">
+        <v>1312</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
@@ -3301,67 +3301,67 @@
       </c>
       <c r="D13" s="9">
         <f t="shared" si="0"/>
-        <v>517.15</v>
-      </c>
-      <c r="E13" s="10">
-        <v>535</v>
-      </c>
-      <c r="F13" s="10">
-        <v>517</v>
-      </c>
-      <c r="G13" s="10">
+        <v>514.70000000000005</v>
+      </c>
+      <c r="E13" s="26">
+        <v>512</v>
+      </c>
+      <c r="F13" s="26">
+        <v>512</v>
+      </c>
+      <c r="G13" s="26">
+        <v>512</v>
+      </c>
+      <c r="H13" s="26">
+        <v>512</v>
+      </c>
+      <c r="I13" s="26">
+        <v>513</v>
+      </c>
+      <c r="J13" s="10">
+        <v>513</v>
+      </c>
+      <c r="K13" s="10">
         <v>514</v>
       </c>
-      <c r="H13" s="10">
-        <v>517</v>
-      </c>
-      <c r="I13" s="10">
+      <c r="L13" s="10">
+        <v>514</v>
+      </c>
+      <c r="M13" s="10">
+        <v>514</v>
+      </c>
+      <c r="N13" s="10">
+        <v>514</v>
+      </c>
+      <c r="O13" s="10">
         <v>515</v>
-      </c>
-      <c r="J13" s="10">
-        <v>512</v>
-      </c>
-      <c r="K13" s="10">
-        <v>512</v>
-      </c>
-      <c r="L13" s="10">
-        <v>513</v>
-      </c>
-      <c r="M13" s="10">
-        <v>532</v>
-      </c>
-      <c r="N13" s="10">
-        <v>513</v>
-      </c>
-      <c r="O13" s="10">
-        <v>518</v>
       </c>
       <c r="P13" s="10">
         <v>515</v>
       </c>
       <c r="Q13" s="10">
+        <v>515</v>
+      </c>
+      <c r="R13" s="10">
+        <v>516</v>
+      </c>
+      <c r="S13" s="10">
+        <v>517</v>
+      </c>
+      <c r="T13" s="26">
+        <v>517</v>
+      </c>
+      <c r="U13" s="26">
+        <v>518</v>
+      </c>
+      <c r="V13" s="26">
+        <v>532</v>
+      </c>
+      <c r="W13" s="27">
         <v>533</v>
       </c>
-      <c r="R13" s="10">
-        <v>514</v>
-      </c>
-      <c r="S13" s="10">
-        <v>515</v>
-      </c>
-      <c r="T13" s="10">
-        <v>512</v>
-      </c>
-      <c r="U13" s="10">
-        <v>512</v>
-      </c>
-      <c r="V13" s="10">
-        <v>514</v>
-      </c>
-      <c r="W13" s="8">
-        <v>514</v>
-      </c>
-      <c r="X13" s="10">
-        <v>516</v>
+      <c r="X13" s="26">
+        <v>535</v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
@@ -3373,46 +3373,46 @@
       </c>
       <c r="D14" s="9">
         <f t="shared" si="0"/>
-        <v>688.9</v>
-      </c>
-      <c r="E14" s="10">
-        <v>705</v>
-      </c>
-      <c r="F14" s="10">
-        <v>690</v>
-      </c>
-      <c r="G14" s="10">
+        <v>686.3</v>
+      </c>
+      <c r="E14" s="26">
         <v>684</v>
       </c>
-      <c r="H14" s="10">
+      <c r="F14" s="26">
+        <v>684</v>
+      </c>
+      <c r="G14" s="26">
+        <v>684</v>
+      </c>
+      <c r="H14" s="26">
+        <v>685</v>
+      </c>
+      <c r="I14" s="26">
+        <v>685</v>
+      </c>
+      <c r="J14" s="10">
+        <v>685</v>
+      </c>
+      <c r="K14" s="10">
+        <v>685</v>
+      </c>
+      <c r="L14" s="10">
+        <v>686</v>
+      </c>
+      <c r="M14" s="10">
+        <v>686</v>
+      </c>
+      <c r="N14" s="10">
+        <v>686</v>
+      </c>
+      <c r="O14" s="10">
         <v>687</v>
-      </c>
-      <c r="I14" s="10">
-        <v>684</v>
-      </c>
-      <c r="J14" s="10">
-        <v>686</v>
-      </c>
-      <c r="K14" s="10">
-        <v>686</v>
-      </c>
-      <c r="L14" s="10">
-        <v>687</v>
-      </c>
-      <c r="M14" s="10">
-        <v>705</v>
-      </c>
-      <c r="N14" s="10">
-        <v>685</v>
-      </c>
-      <c r="O14" s="10">
-        <v>689</v>
       </c>
       <c r="P14" s="10">
         <v>687</v>
       </c>
       <c r="Q14" s="10">
-        <v>704</v>
+        <v>687</v>
       </c>
       <c r="R14" s="10">
         <v>687</v>
@@ -3420,20 +3420,20 @@
       <c r="S14" s="10">
         <v>687</v>
       </c>
-      <c r="T14" s="10">
-        <v>685</v>
-      </c>
-      <c r="U14" s="10">
-        <v>685</v>
-      </c>
-      <c r="V14" s="10">
-        <v>684</v>
-      </c>
-      <c r="W14" s="8">
-        <v>686</v>
-      </c>
-      <c r="X14" s="10">
-        <v>685</v>
+      <c r="T14" s="26">
+        <v>689</v>
+      </c>
+      <c r="U14" s="26">
+        <v>690</v>
+      </c>
+      <c r="V14" s="26">
+        <v>704</v>
+      </c>
+      <c r="W14" s="27">
+        <v>705</v>
+      </c>
+      <c r="X14" s="26">
+        <v>705</v>
       </c>
     </row>
     <row r="15" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3445,67 +3445,67 @@
       </c>
       <c r="D15" s="9">
         <f t="shared" si="0"/>
-        <v>1291.25</v>
-      </c>
-      <c r="E15" s="10">
-        <v>1307</v>
-      </c>
-      <c r="F15" s="10">
-        <v>1288</v>
-      </c>
-      <c r="G15" s="10">
+        <v>1287.5</v>
+      </c>
+      <c r="E15" s="26">
+        <v>1285</v>
+      </c>
+      <c r="F15" s="26">
+        <v>1285</v>
+      </c>
+      <c r="G15" s="26">
         <v>1286</v>
       </c>
-      <c r="H15" s="10">
-        <v>1289</v>
-      </c>
-      <c r="I15" s="10">
-        <v>1287</v>
+      <c r="H15" s="26">
+        <v>1286</v>
+      </c>
+      <c r="I15" s="26">
+        <v>1286</v>
       </c>
       <c r="J15" s="10">
         <v>1286</v>
       </c>
       <c r="K15" s="10">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="L15" s="10">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="M15" s="10">
-        <v>1330</v>
+        <v>1287</v>
       </c>
       <c r="N15" s="10">
         <v>1287</v>
       </c>
       <c r="O15" s="10">
+        <v>1288</v>
+      </c>
+      <c r="P15" s="10">
+        <v>1288</v>
+      </c>
+      <c r="Q15" s="10">
+        <v>1288</v>
+      </c>
+      <c r="R15" s="10">
+        <v>1289</v>
+      </c>
+      <c r="S15" s="10">
+        <v>1289</v>
+      </c>
+      <c r="T15" s="26">
+        <v>1289</v>
+      </c>
+      <c r="U15" s="26">
         <v>1291</v>
       </c>
-      <c r="P15" s="10">
-        <v>1285</v>
-      </c>
-      <c r="Q15" s="10">
+      <c r="V15" s="26">
         <v>1305</v>
       </c>
-      <c r="R15" s="10">
-        <v>1285</v>
-      </c>
-      <c r="S15" s="10">
-        <v>1286</v>
-      </c>
-      <c r="T15" s="10">
-        <v>1286</v>
-      </c>
-      <c r="U15" s="10">
-        <v>1288</v>
-      </c>
-      <c r="V15" s="10">
-        <v>1287</v>
-      </c>
-      <c r="W15" s="8">
-        <v>1286</v>
-      </c>
-      <c r="X15" s="10">
-        <v>1289</v>
+      <c r="W15" s="27">
+        <v>1307</v>
+      </c>
+      <c r="X15" s="26">
+        <v>1330</v>
       </c>
     </row>
     <row r="17" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3523,19 +3523,19 @@
       <c r="D18" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="23">
         <v>1</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="23">
         <v>2</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="23">
         <v>3</v>
       </c>
-      <c r="H18" s="17">
+      <c r="H18" s="23">
         <v>4</v>
       </c>
-      <c r="I18" s="17">
+      <c r="I18" s="23">
         <v>5</v>
       </c>
       <c r="J18" s="17">
@@ -3568,19 +3568,19 @@
       <c r="S18" s="17">
         <v>15</v>
       </c>
-      <c r="T18" s="17">
+      <c r="T18" s="23">
         <v>16</v>
       </c>
-      <c r="U18" s="17">
+      <c r="U18" s="23">
         <v>17</v>
       </c>
-      <c r="V18" s="17">
+      <c r="V18" s="23">
         <v>18</v>
       </c>
-      <c r="W18" s="16">
+      <c r="W18" s="24">
         <v>19</v>
       </c>
-      <c r="X18" s="17">
+      <c r="X18" s="23">
         <v>20</v>
       </c>
     </row>
@@ -3592,22 +3592,22 @@
         <v>1</v>
       </c>
       <c r="D19" s="3">
-        <f>AVERAGE(E19:AC19)</f>
-        <v>261</v>
-      </c>
-      <c r="E19" s="3">
-        <v>261</v>
-      </c>
-      <c r="F19" s="3">
-        <v>261</v>
-      </c>
-      <c r="G19" s="3">
-        <v>261</v>
-      </c>
-      <c r="H19" s="3">
-        <v>261</v>
-      </c>
-      <c r="I19" s="3">
+        <f>AVERAGE(J19:S19)</f>
+        <v>261</v>
+      </c>
+      <c r="E19" s="18">
+        <v>261</v>
+      </c>
+      <c r="F19" s="18">
+        <v>261</v>
+      </c>
+      <c r="G19" s="18">
+        <v>261</v>
+      </c>
+      <c r="H19" s="18">
+        <v>261</v>
+      </c>
+      <c r="I19" s="18">
         <v>261</v>
       </c>
       <c r="J19" s="3">
@@ -3640,19 +3640,19 @@
       <c r="S19" s="3">
         <v>261</v>
       </c>
-      <c r="T19" s="3">
-        <v>261</v>
-      </c>
-      <c r="U19" s="3">
-        <v>261</v>
-      </c>
-      <c r="V19" s="3">
-        <v>261</v>
-      </c>
-      <c r="W19" s="3">
-        <v>261</v>
-      </c>
-      <c r="X19" s="3">
+      <c r="T19" s="18">
+        <v>261</v>
+      </c>
+      <c r="U19" s="18">
+        <v>261</v>
+      </c>
+      <c r="V19" s="18">
+        <v>261</v>
+      </c>
+      <c r="W19" s="18">
+        <v>261</v>
+      </c>
+      <c r="X19" s="18">
         <v>261</v>
       </c>
     </row>
@@ -3664,22 +3664,22 @@
         <v>2</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" ref="D20:D30" si="1">AVERAGE(E20:AC20)</f>
-        <v>476</v>
-      </c>
-      <c r="E20" s="6">
-        <v>476</v>
-      </c>
-      <c r="F20" s="6">
-        <v>476</v>
-      </c>
-      <c r="G20" s="6">
-        <v>476</v>
-      </c>
-      <c r="H20" s="6">
-        <v>476</v>
-      </c>
-      <c r="I20" s="6">
+        <f t="shared" ref="D20:D30" si="1">AVERAGE(J20:S20)</f>
+        <v>476</v>
+      </c>
+      <c r="E20" s="19">
+        <v>476</v>
+      </c>
+      <c r="F20" s="19">
+        <v>476</v>
+      </c>
+      <c r="G20" s="19">
+        <v>476</v>
+      </c>
+      <c r="H20" s="19">
+        <v>476</v>
+      </c>
+      <c r="I20" s="19">
         <v>476</v>
       </c>
       <c r="J20" s="6">
@@ -3712,19 +3712,19 @@
       <c r="S20" s="6">
         <v>476</v>
       </c>
-      <c r="T20" s="6">
-        <v>476</v>
-      </c>
-      <c r="U20" s="6">
-        <v>476</v>
-      </c>
-      <c r="V20" s="6">
-        <v>476</v>
-      </c>
-      <c r="W20" s="6">
-        <v>476</v>
-      </c>
-      <c r="X20" s="6">
+      <c r="T20" s="19">
+        <v>476</v>
+      </c>
+      <c r="U20" s="19">
+        <v>476</v>
+      </c>
+      <c r="V20" s="19">
+        <v>476</v>
+      </c>
+      <c r="W20" s="19">
+        <v>476</v>
+      </c>
+      <c r="X20" s="19">
         <v>476</v>
       </c>
     </row>
@@ -3739,19 +3739,19 @@
         <f t="shared" si="1"/>
         <v>1330</v>
       </c>
-      <c r="E21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="F21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="G21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="H21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="I21" s="6">
+      <c r="E21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="F21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="G21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="H21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="I21" s="19">
         <v>1330</v>
       </c>
       <c r="J21" s="6">
@@ -3784,19 +3784,19 @@
       <c r="S21" s="6">
         <v>1330</v>
       </c>
-      <c r="T21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="U21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="V21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="W21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="X21" s="6">
+      <c r="T21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="U21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="V21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="W21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="X21" s="19">
         <v>1330</v>
       </c>
     </row>
@@ -3811,19 +3811,19 @@
         <f t="shared" si="1"/>
         <v>261</v>
       </c>
-      <c r="E22" s="10">
-        <v>261</v>
-      </c>
-      <c r="F22" s="10">
-        <v>261</v>
-      </c>
-      <c r="G22" s="10">
-        <v>261</v>
-      </c>
-      <c r="H22" s="10">
-        <v>261</v>
-      </c>
-      <c r="I22" s="10">
+      <c r="E22" s="26">
+        <v>261</v>
+      </c>
+      <c r="F22" s="26">
+        <v>261</v>
+      </c>
+      <c r="G22" s="26">
+        <v>261</v>
+      </c>
+      <c r="H22" s="26">
+        <v>261</v>
+      </c>
+      <c r="I22" s="26">
         <v>261</v>
       </c>
       <c r="J22" s="10">
@@ -3856,19 +3856,19 @@
       <c r="S22" s="10">
         <v>261</v>
       </c>
-      <c r="T22" s="10">
-        <v>261</v>
-      </c>
-      <c r="U22" s="10">
-        <v>261</v>
-      </c>
-      <c r="V22" s="10">
-        <v>261</v>
-      </c>
-      <c r="W22" s="10">
-        <v>261</v>
-      </c>
-      <c r="X22" s="10">
+      <c r="T22" s="26">
+        <v>261</v>
+      </c>
+      <c r="U22" s="26">
+        <v>261</v>
+      </c>
+      <c r="V22" s="26">
+        <v>261</v>
+      </c>
+      <c r="W22" s="26">
+        <v>261</v>
+      </c>
+      <c r="X22" s="26">
         <v>261</v>
       </c>
     </row>
@@ -3883,19 +3883,19 @@
         <f t="shared" si="1"/>
         <v>476</v>
       </c>
-      <c r="E23" s="10">
-        <v>476</v>
-      </c>
-      <c r="F23" s="10">
-        <v>476</v>
-      </c>
-      <c r="G23" s="10">
-        <v>476</v>
-      </c>
-      <c r="H23" s="10">
-        <v>476</v>
-      </c>
-      <c r="I23" s="10">
+      <c r="E23" s="26">
+        <v>476</v>
+      </c>
+      <c r="F23" s="26">
+        <v>476</v>
+      </c>
+      <c r="G23" s="26">
+        <v>476</v>
+      </c>
+      <c r="H23" s="26">
+        <v>476</v>
+      </c>
+      <c r="I23" s="26">
         <v>476</v>
       </c>
       <c r="J23" s="10">
@@ -3928,19 +3928,19 @@
       <c r="S23" s="10">
         <v>476</v>
       </c>
-      <c r="T23" s="10">
-        <v>476</v>
-      </c>
-      <c r="U23" s="10">
-        <v>476</v>
-      </c>
-      <c r="V23" s="10">
-        <v>476</v>
-      </c>
-      <c r="W23" s="10">
-        <v>476</v>
-      </c>
-      <c r="X23" s="10">
+      <c r="T23" s="26">
+        <v>476</v>
+      </c>
+      <c r="U23" s="26">
+        <v>476</v>
+      </c>
+      <c r="V23" s="26">
+        <v>476</v>
+      </c>
+      <c r="W23" s="26">
+        <v>476</v>
+      </c>
+      <c r="X23" s="26">
         <v>476</v>
       </c>
     </row>
@@ -3955,19 +3955,19 @@
         <f t="shared" si="1"/>
         <v>1330</v>
       </c>
-      <c r="E24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="F24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="G24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="H24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="I24" s="10">
+      <c r="E24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="F24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="G24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="H24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="I24" s="26">
         <v>1330</v>
       </c>
       <c r="J24" s="10">
@@ -4000,19 +4000,19 @@
       <c r="S24" s="10">
         <v>1330</v>
       </c>
-      <c r="T24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="U24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="V24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="W24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="X24" s="10">
+      <c r="T24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="U24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="V24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="W24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="X24" s="26">
         <v>1330</v>
       </c>
     </row>
@@ -4027,19 +4027,19 @@
         <f t="shared" si="1"/>
         <v>261</v>
       </c>
-      <c r="E25" s="6">
-        <v>261</v>
-      </c>
-      <c r="F25" s="6">
-        <v>261</v>
-      </c>
-      <c r="G25" s="6">
-        <v>261</v>
-      </c>
-      <c r="H25" s="6">
-        <v>261</v>
-      </c>
-      <c r="I25" s="6">
+      <c r="E25" s="19">
+        <v>261</v>
+      </c>
+      <c r="F25" s="19">
+        <v>261</v>
+      </c>
+      <c r="G25" s="19">
+        <v>261</v>
+      </c>
+      <c r="H25" s="19">
+        <v>261</v>
+      </c>
+      <c r="I25" s="19">
         <v>261</v>
       </c>
       <c r="J25" s="6">
@@ -4072,19 +4072,19 @@
       <c r="S25" s="6">
         <v>261</v>
       </c>
-      <c r="T25" s="6">
-        <v>261</v>
-      </c>
-      <c r="U25" s="6">
-        <v>261</v>
-      </c>
-      <c r="V25" s="6">
-        <v>261</v>
-      </c>
-      <c r="W25" s="6">
-        <v>261</v>
-      </c>
-      <c r="X25" s="6">
+      <c r="T25" s="19">
+        <v>261</v>
+      </c>
+      <c r="U25" s="19">
+        <v>261</v>
+      </c>
+      <c r="V25" s="19">
+        <v>261</v>
+      </c>
+      <c r="W25" s="19">
+        <v>261</v>
+      </c>
+      <c r="X25" s="19">
         <v>261</v>
       </c>
     </row>
@@ -4099,19 +4099,19 @@
         <f t="shared" si="1"/>
         <v>476</v>
       </c>
-      <c r="E26" s="6">
-        <v>476</v>
-      </c>
-      <c r="F26" s="6">
-        <v>476</v>
-      </c>
-      <c r="G26" s="6">
-        <v>476</v>
-      </c>
-      <c r="H26" s="6">
-        <v>476</v>
-      </c>
-      <c r="I26" s="6">
+      <c r="E26" s="19">
+        <v>476</v>
+      </c>
+      <c r="F26" s="19">
+        <v>476</v>
+      </c>
+      <c r="G26" s="19">
+        <v>476</v>
+      </c>
+      <c r="H26" s="19">
+        <v>476</v>
+      </c>
+      <c r="I26" s="19">
         <v>476</v>
       </c>
       <c r="J26" s="6">
@@ -4144,19 +4144,19 @@
       <c r="S26" s="6">
         <v>476</v>
       </c>
-      <c r="T26" s="6">
-        <v>476</v>
-      </c>
-      <c r="U26" s="6">
-        <v>476</v>
-      </c>
-      <c r="V26" s="6">
-        <v>476</v>
-      </c>
-      <c r="W26" s="6">
-        <v>476</v>
-      </c>
-      <c r="X26" s="6">
+      <c r="T26" s="19">
+        <v>476</v>
+      </c>
+      <c r="U26" s="19">
+        <v>476</v>
+      </c>
+      <c r="V26" s="19">
+        <v>476</v>
+      </c>
+      <c r="W26" s="19">
+        <v>476</v>
+      </c>
+      <c r="X26" s="19">
         <v>476</v>
       </c>
     </row>
@@ -4171,19 +4171,19 @@
         <f t="shared" si="1"/>
         <v>1330</v>
       </c>
-      <c r="E27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="F27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="G27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="H27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="I27" s="6">
+      <c r="E27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="F27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="G27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="H27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="I27" s="19">
         <v>1330</v>
       </c>
       <c r="J27" s="6">
@@ -4216,19 +4216,19 @@
       <c r="S27" s="6">
         <v>1330</v>
       </c>
-      <c r="T27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="U27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="V27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="W27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="X27" s="6">
+      <c r="T27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="U27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="V27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="W27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="X27" s="19">
         <v>1330</v>
       </c>
     </row>
@@ -4243,19 +4243,19 @@
         <f t="shared" si="1"/>
         <v>261</v>
       </c>
-      <c r="E28" s="10">
-        <v>261</v>
-      </c>
-      <c r="F28" s="10">
-        <v>261</v>
-      </c>
-      <c r="G28" s="10">
-        <v>261</v>
-      </c>
-      <c r="H28" s="10">
-        <v>261</v>
-      </c>
-      <c r="I28" s="10">
+      <c r="E28" s="26">
+        <v>261</v>
+      </c>
+      <c r="F28" s="26">
+        <v>261</v>
+      </c>
+      <c r="G28" s="26">
+        <v>261</v>
+      </c>
+      <c r="H28" s="26">
+        <v>261</v>
+      </c>
+      <c r="I28" s="26">
         <v>261</v>
       </c>
       <c r="J28" s="10">
@@ -4288,19 +4288,19 @@
       <c r="S28" s="10">
         <v>261</v>
       </c>
-      <c r="T28" s="10">
-        <v>261</v>
-      </c>
-      <c r="U28" s="10">
-        <v>261</v>
-      </c>
-      <c r="V28" s="10">
-        <v>261</v>
-      </c>
-      <c r="W28" s="10">
-        <v>261</v>
-      </c>
-      <c r="X28" s="10">
+      <c r="T28" s="26">
+        <v>261</v>
+      </c>
+      <c r="U28" s="26">
+        <v>261</v>
+      </c>
+      <c r="V28" s="26">
+        <v>261</v>
+      </c>
+      <c r="W28" s="26">
+        <v>261</v>
+      </c>
+      <c r="X28" s="26">
         <v>261</v>
       </c>
     </row>
@@ -4315,19 +4315,19 @@
         <f t="shared" si="1"/>
         <v>476</v>
       </c>
-      <c r="E29" s="10">
-        <v>476</v>
-      </c>
-      <c r="F29" s="10">
-        <v>476</v>
-      </c>
-      <c r="G29" s="10">
-        <v>476</v>
-      </c>
-      <c r="H29" s="10">
-        <v>476</v>
-      </c>
-      <c r="I29" s="10">
+      <c r="E29" s="26">
+        <v>476</v>
+      </c>
+      <c r="F29" s="26">
+        <v>476</v>
+      </c>
+      <c r="G29" s="26">
+        <v>476</v>
+      </c>
+      <c r="H29" s="26">
+        <v>476</v>
+      </c>
+      <c r="I29" s="26">
         <v>476</v>
       </c>
       <c r="J29" s="10">
@@ -4360,19 +4360,19 @@
       <c r="S29" s="10">
         <v>476</v>
       </c>
-      <c r="T29" s="10">
-        <v>476</v>
-      </c>
-      <c r="U29" s="10">
-        <v>476</v>
-      </c>
-      <c r="V29" s="10">
-        <v>476</v>
-      </c>
-      <c r="W29" s="10">
-        <v>476</v>
-      </c>
-      <c r="X29" s="10">
+      <c r="T29" s="26">
+        <v>476</v>
+      </c>
+      <c r="U29" s="26">
+        <v>476</v>
+      </c>
+      <c r="V29" s="26">
+        <v>476</v>
+      </c>
+      <c r="W29" s="26">
+        <v>476</v>
+      </c>
+      <c r="X29" s="26">
         <v>476</v>
       </c>
     </row>
@@ -4387,19 +4387,19 @@
         <f t="shared" si="1"/>
         <v>1330</v>
       </c>
-      <c r="E30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="F30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="G30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="H30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="I30" s="10">
+      <c r="E30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="F30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="G30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="H30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="I30" s="26">
         <v>1330</v>
       </c>
       <c r="J30" s="10">
@@ -4432,23 +4432,26 @@
       <c r="S30" s="10">
         <v>1330</v>
       </c>
-      <c r="T30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="U30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="V30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="W30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="X30" s="10">
+      <c r="T30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="U30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="V30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="W30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="X30" s="26">
         <v>1330</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="E15:X15">
+    <sortCondition ref="E15:X15"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Sorted GTAO memory measurements
</commit_message>
<xml_diff>
--- a/Experiment/Results/MemoryUsageSorted.xlsx
+++ b/Experiment/Results/MemoryUsageSorted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Howest\GD_J3_S2\Gradwork_2.0\Gradwork\Experiment\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91E80E0-0573-4F90-AF21-3C1809B77ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B40A89-8DBA-4C55-BC95-7D071369BE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10790" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-10790" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SSAO" sheetId="1" r:id="rId1"/>
@@ -2556,8 +2556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051415FD-3633-4903-A550-646AFA39BC19}">
   <dimension ref="B2:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4461,8 +4461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F9889E-C474-4008-911C-31263606DEAC}">
   <dimension ref="B2:X30"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4487,19 +4487,19 @@
       <c r="D3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="23">
         <v>1</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="23">
         <v>2</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="23">
         <v>3</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="23">
         <v>4</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="23">
         <v>5</v>
       </c>
       <c r="J3" s="17">
@@ -4532,19 +4532,19 @@
       <c r="S3" s="17">
         <v>15</v>
       </c>
-      <c r="T3" s="17">
+      <c r="T3" s="23">
         <v>16</v>
       </c>
-      <c r="U3" s="17">
+      <c r="U3" s="23">
         <v>17</v>
       </c>
-      <c r="V3" s="17">
+      <c r="V3" s="23">
         <v>18</v>
       </c>
-      <c r="W3" s="16">
+      <c r="W3" s="24">
         <v>19</v>
       </c>
-      <c r="X3" s="17">
+      <c r="X3" s="23">
         <v>20</v>
       </c>
     </row>
@@ -4556,68 +4556,68 @@
         <v>1</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D4:D15" si="0">AVERAGE(E4:AC4)</f>
-        <v>516.70000000000005</v>
-      </c>
-      <c r="E4" s="3">
-        <v>528</v>
-      </c>
-      <c r="F4" s="3">
-        <v>521</v>
-      </c>
-      <c r="G4" s="3">
+        <f>AVERAGE(J4:S4)</f>
+        <v>515.6</v>
+      </c>
+      <c r="E4" s="18">
+        <v>512</v>
+      </c>
+      <c r="F4" s="18">
+        <v>512</v>
+      </c>
+      <c r="G4" s="18">
         <v>513</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="18">
+        <v>513</v>
+      </c>
+      <c r="I4" s="18">
         <v>514</v>
       </c>
-      <c r="I4" s="3">
-        <v>525</v>
-      </c>
       <c r="J4" s="3">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="K4" s="3">
         <v>515</v>
       </c>
       <c r="L4" s="3">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="M4" s="3">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="N4" s="3">
+        <v>515</v>
+      </c>
+      <c r="O4" s="3">
+        <v>515</v>
+      </c>
+      <c r="P4" s="3">
         <v>516</v>
-      </c>
-      <c r="O4" s="3">
-        <v>514</v>
-      </c>
-      <c r="P4" s="3">
-        <v>512</v>
       </c>
       <c r="Q4" s="3">
         <v>517</v>
       </c>
       <c r="R4" s="3">
-        <v>512</v>
+        <v>517</v>
       </c>
       <c r="S4" s="3">
-        <v>513</v>
-      </c>
-      <c r="T4" s="3">
-        <v>515</v>
-      </c>
-      <c r="U4" s="3">
         <v>517</v>
       </c>
-      <c r="V4" s="3">
+      <c r="T4" s="18">
+        <v>518</v>
+      </c>
+      <c r="U4" s="18">
+        <v>521</v>
+      </c>
+      <c r="V4" s="18">
         <v>522</v>
       </c>
-      <c r="W4" s="2">
-        <v>515</v>
-      </c>
-      <c r="X4" s="3">
-        <v>515</v>
+      <c r="W4" s="21">
+        <v>525</v>
+      </c>
+      <c r="X4" s="18">
+        <v>528</v>
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.3">
@@ -4628,35 +4628,35 @@
         <v>2</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="0"/>
-        <v>687.2</v>
-      </c>
-      <c r="E5" s="6">
-        <v>700</v>
-      </c>
-      <c r="F5" s="6">
+        <f t="shared" ref="D5:D15" si="0">AVERAGE(J5:S5)</f>
+        <v>686.5</v>
+      </c>
+      <c r="E5" s="19">
+        <v>684</v>
+      </c>
+      <c r="F5" s="19">
+        <v>684</v>
+      </c>
+      <c r="G5" s="19">
         <v>685</v>
       </c>
-      <c r="G5" s="6">
-        <v>684</v>
-      </c>
-      <c r="H5" s="6">
+      <c r="H5" s="19">
+        <v>685</v>
+      </c>
+      <c r="I5" s="19">
+        <v>685</v>
+      </c>
+      <c r="J5" s="6">
+        <v>685</v>
+      </c>
+      <c r="K5" s="6">
         <v>686</v>
       </c>
-      <c r="I5" s="6">
-        <v>688</v>
-      </c>
-      <c r="J5" s="6">
-        <v>687</v>
-      </c>
-      <c r="K5" s="6">
-        <v>687</v>
-      </c>
       <c r="L5" s="6">
-        <v>692</v>
+        <v>686</v>
       </c>
       <c r="M5" s="6">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="N5" s="6">
         <v>687</v>
@@ -4665,31 +4665,31 @@
         <v>687</v>
       </c>
       <c r="P5" s="6">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="Q5" s="6">
         <v>687</v>
       </c>
       <c r="R5" s="6">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="S5" s="6">
-        <v>685</v>
-      </c>
-      <c r="T5" s="6">
         <v>687</v>
       </c>
-      <c r="U5" s="6">
-        <v>686</v>
-      </c>
-      <c r="V5" s="6">
+      <c r="T5" s="19">
         <v>687</v>
       </c>
-      <c r="W5" s="5">
-        <v>685</v>
-      </c>
-      <c r="X5" s="6">
-        <v>686</v>
+      <c r="U5" s="19">
+        <v>688</v>
+      </c>
+      <c r="V5" s="19">
+        <v>689</v>
+      </c>
+      <c r="W5" s="22">
+        <v>692</v>
+      </c>
+      <c r="X5" s="19">
+        <v>700</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
@@ -4701,31 +4701,31 @@
       </c>
       <c r="D6" s="3">
         <f t="shared" si="0"/>
-        <v>1290.75</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1302</v>
-      </c>
-      <c r="F6" s="6">
+        <v>1287.9000000000001</v>
+      </c>
+      <c r="E6" s="19">
+        <v>1284</v>
+      </c>
+      <c r="F6" s="19">
+        <v>1285</v>
+      </c>
+      <c r="G6" s="19">
+        <v>1285</v>
+      </c>
+      <c r="H6" s="19">
         <v>1286</v>
       </c>
-      <c r="G6" s="6">
-        <v>1284</v>
-      </c>
-      <c r="H6" s="6">
-        <v>1289</v>
-      </c>
-      <c r="I6" s="6">
+      <c r="I6" s="19">
+        <v>1286</v>
+      </c>
+      <c r="J6" s="6">
         <v>1287</v>
       </c>
-      <c r="J6" s="6">
-        <v>1305</v>
-      </c>
       <c r="K6" s="6">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="L6" s="6">
-        <v>1290</v>
+        <v>1287</v>
       </c>
       <c r="M6" s="6">
         <v>1287</v>
@@ -4734,33 +4734,33 @@
         <v>1288</v>
       </c>
       <c r="O6" s="6">
-        <v>1305</v>
+        <v>1288</v>
       </c>
       <c r="P6" s="6">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="Q6" s="6">
         <v>1288</v>
       </c>
       <c r="R6" s="6">
-        <v>1285</v>
+        <v>1289</v>
       </c>
       <c r="S6" s="6">
-        <v>1286</v>
-      </c>
-      <c r="T6" s="6">
-        <v>1287</v>
-      </c>
-      <c r="U6" s="6">
-        <v>1288</v>
-      </c>
-      <c r="V6" s="6">
         <v>1290</v>
       </c>
-      <c r="W6" s="5">
-        <v>1285</v>
-      </c>
-      <c r="X6" s="6">
+      <c r="T6" s="19">
+        <v>1290</v>
+      </c>
+      <c r="U6" s="19">
+        <v>1302</v>
+      </c>
+      <c r="V6" s="19">
+        <v>1305</v>
+      </c>
+      <c r="W6" s="22">
+        <v>1305</v>
+      </c>
+      <c r="X6" s="19">
         <v>1308</v>
       </c>
     </row>
@@ -4773,28 +4773,28 @@
       </c>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
-        <v>516.25</v>
-      </c>
-      <c r="E7" s="10">
-        <v>526</v>
-      </c>
-      <c r="F7" s="10">
-        <v>517</v>
-      </c>
-      <c r="G7" s="10">
-        <v>516</v>
-      </c>
-      <c r="H7" s="10">
-        <v>516</v>
-      </c>
-      <c r="I7" s="10">
-        <v>519</v>
+        <v>515.6</v>
+      </c>
+      <c r="E7" s="26">
+        <v>512</v>
+      </c>
+      <c r="F7" s="26">
+        <v>513</v>
+      </c>
+      <c r="G7" s="26">
+        <v>513</v>
+      </c>
+      <c r="H7" s="26">
+        <v>514</v>
+      </c>
+      <c r="I7" s="26">
+        <v>514</v>
       </c>
       <c r="J7" s="10">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="K7" s="10">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="L7" s="10">
         <v>515</v>
@@ -4803,37 +4803,37 @@
         <v>515</v>
       </c>
       <c r="N7" s="10">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="O7" s="10">
         <v>516</v>
       </c>
       <c r="P7" s="10">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="Q7" s="10">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="R7" s="10">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="S7" s="10">
         <v>518</v>
       </c>
-      <c r="T7" s="10">
-        <v>514</v>
-      </c>
-      <c r="U7" s="10">
-        <v>514</v>
-      </c>
-      <c r="V7" s="10">
-        <v>514</v>
-      </c>
-      <c r="W7" s="8">
+      <c r="T7" s="26">
         <v>518</v>
       </c>
-      <c r="X7" s="10">
-        <v>514</v>
+      <c r="U7" s="26">
+        <v>519</v>
+      </c>
+      <c r="V7" s="26">
+        <v>519</v>
+      </c>
+      <c r="W7" s="27">
+        <v>521</v>
+      </c>
+      <c r="X7" s="26">
+        <v>526</v>
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
@@ -4845,37 +4845,37 @@
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
-        <v>693</v>
-      </c>
-      <c r="E8" s="10">
-        <v>704</v>
-      </c>
-      <c r="F8" s="10">
+        <v>690.7</v>
+      </c>
+      <c r="E8" s="26">
+        <v>685</v>
+      </c>
+      <c r="F8" s="26">
+        <v>685</v>
+      </c>
+      <c r="G8" s="26">
+        <v>685</v>
+      </c>
+      <c r="H8" s="26">
+        <v>686</v>
+      </c>
+      <c r="I8" s="26">
+        <v>686</v>
+      </c>
+      <c r="J8" s="10">
         <v>687</v>
       </c>
-      <c r="G8" s="10">
-        <v>707</v>
-      </c>
-      <c r="H8" s="10">
-        <v>706</v>
-      </c>
-      <c r="I8" s="10">
+      <c r="K8" s="10">
+        <v>687</v>
+      </c>
+      <c r="L8" s="10">
+        <v>687</v>
+      </c>
+      <c r="M8" s="10">
+        <v>687</v>
+      </c>
+      <c r="N8" s="10">
         <v>688</v>
-      </c>
-      <c r="J8" s="10">
-        <v>685</v>
-      </c>
-      <c r="K8" s="10">
-        <v>704</v>
-      </c>
-      <c r="L8" s="10">
-        <v>686</v>
-      </c>
-      <c r="M8" s="10">
-        <v>685</v>
-      </c>
-      <c r="N8" s="10">
-        <v>685</v>
       </c>
       <c r="O8" s="10">
         <v>688</v>
@@ -4884,28 +4884,28 @@
         <v>688</v>
       </c>
       <c r="Q8" s="10">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="R8" s="10">
-        <v>686</v>
+        <v>702</v>
       </c>
       <c r="S8" s="10">
-        <v>687</v>
-      </c>
-      <c r="T8" s="10">
+        <v>704</v>
+      </c>
+      <c r="T8" s="26">
+        <v>704</v>
+      </c>
+      <c r="U8" s="26">
+        <v>704</v>
+      </c>
+      <c r="V8" s="26">
         <v>705</v>
       </c>
-      <c r="U8" s="10">
-        <v>702</v>
-      </c>
-      <c r="V8" s="10">
-        <v>687</v>
-      </c>
-      <c r="W8" s="8">
-        <v>689</v>
-      </c>
-      <c r="X8" s="10">
-        <v>704</v>
+      <c r="W8" s="27">
+        <v>706</v>
+      </c>
+      <c r="X8" s="26">
+        <v>707</v>
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
@@ -4917,67 +4917,67 @@
       </c>
       <c r="D9" s="9">
         <f t="shared" si="0"/>
-        <v>1296.4000000000001</v>
-      </c>
-      <c r="E9" s="10">
-        <v>1305</v>
-      </c>
-      <c r="F9" s="10">
-        <v>1308</v>
-      </c>
-      <c r="G9" s="10">
-        <v>1305</v>
-      </c>
-      <c r="H9" s="10">
-        <v>1307</v>
-      </c>
-      <c r="I9" s="10">
+        <v>1295.9000000000001</v>
+      </c>
+      <c r="E9" s="26">
+        <v>1285</v>
+      </c>
+      <c r="F9" s="26">
+        <v>1287</v>
+      </c>
+      <c r="G9" s="26">
+        <v>1287</v>
+      </c>
+      <c r="H9" s="26">
+        <v>1287</v>
+      </c>
+      <c r="I9" s="26">
         <v>1288</v>
       </c>
       <c r="J9" s="10">
         <v>1288</v>
       </c>
       <c r="K9" s="10">
+        <v>1288</v>
+      </c>
+      <c r="L9" s="10">
+        <v>1288</v>
+      </c>
+      <c r="M9" s="10">
+        <v>1289</v>
+      </c>
+      <c r="N9" s="10">
+        <v>1290</v>
+      </c>
+      <c r="O9" s="10">
+        <v>1298</v>
+      </c>
+      <c r="P9" s="10">
         <v>1304</v>
       </c>
-      <c r="L9" s="10">
-        <v>1285</v>
-      </c>
-      <c r="M9" s="10">
-        <v>1288</v>
-      </c>
-      <c r="N9" s="10">
-        <v>1287</v>
-      </c>
-      <c r="O9" s="10">
-        <v>1287</v>
-      </c>
-      <c r="P9" s="10">
-        <v>1287</v>
-      </c>
       <c r="Q9" s="10">
-        <v>1290</v>
+        <v>1304</v>
       </c>
       <c r="R9" s="10">
+        <v>1305</v>
+      </c>
+      <c r="S9" s="10">
+        <v>1305</v>
+      </c>
+      <c r="T9" s="26">
+        <v>1305</v>
+      </c>
+      <c r="U9" s="26">
         <v>1307</v>
       </c>
-      <c r="S9" s="10">
-        <v>1289</v>
-      </c>
-      <c r="T9" s="10">
+      <c r="V9" s="26">
+        <v>1307</v>
+      </c>
+      <c r="W9" s="27">
         <v>1308</v>
       </c>
-      <c r="U9" s="10">
-        <v>1304</v>
-      </c>
-      <c r="V9" s="10">
-        <v>1298</v>
-      </c>
-      <c r="W9" s="8">
-        <v>1288</v>
-      </c>
-      <c r="X9" s="10">
-        <v>1305</v>
+      <c r="X9" s="26">
+        <v>1308</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
@@ -4989,67 +4989,67 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" si="0"/>
-        <v>521</v>
-      </c>
-      <c r="E10" s="6">
-        <v>536</v>
-      </c>
-      <c r="F10" s="6">
+        <v>518.29999999999995</v>
+      </c>
+      <c r="E10" s="19">
+        <v>512</v>
+      </c>
+      <c r="F10" s="19">
         <v>513</v>
       </c>
-      <c r="G10" s="6">
-        <v>533</v>
-      </c>
-      <c r="H10" s="6">
-        <v>523</v>
-      </c>
-      <c r="I10" s="6">
-        <v>517</v>
+      <c r="G10" s="19">
+        <v>513</v>
+      </c>
+      <c r="H10" s="19">
+        <v>513</v>
+      </c>
+      <c r="I10" s="19">
+        <v>513</v>
       </c>
       <c r="J10" s="6">
         <v>513</v>
       </c>
       <c r="K10" s="6">
+        <v>514</v>
+      </c>
+      <c r="L10" s="6">
+        <v>515</v>
+      </c>
+      <c r="M10" s="6">
+        <v>516</v>
+      </c>
+      <c r="N10" s="6">
+        <v>517</v>
+      </c>
+      <c r="O10" s="6">
+        <v>517</v>
+      </c>
+      <c r="P10" s="6">
+        <v>517</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>519</v>
+      </c>
+      <c r="R10" s="6">
+        <v>523</v>
+      </c>
+      <c r="S10" s="6">
+        <v>532</v>
+      </c>
+      <c r="T10" s="19">
+        <v>533</v>
+      </c>
+      <c r="U10" s="19">
+        <v>533</v>
+      </c>
+      <c r="V10" s="19">
         <v>534</v>
       </c>
-      <c r="L10" s="6">
-        <v>532</v>
-      </c>
-      <c r="M10" s="6">
-        <v>517</v>
-      </c>
-      <c r="N10" s="6">
-        <v>519</v>
-      </c>
-      <c r="O10" s="6">
-        <v>533</v>
-      </c>
-      <c r="P10" s="6">
-        <v>516</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>513</v>
-      </c>
-      <c r="R10" s="6">
-        <v>517</v>
-      </c>
-      <c r="S10" s="6">
-        <v>512</v>
-      </c>
-      <c r="T10" s="6">
-        <v>513</v>
-      </c>
-      <c r="U10" s="6">
-        <v>514</v>
-      </c>
-      <c r="V10" s="6">
-        <v>513</v>
-      </c>
-      <c r="W10" s="5">
+      <c r="W10" s="22">
+        <v>536</v>
+      </c>
+      <c r="X10" s="19">
         <v>537</v>
-      </c>
-      <c r="X10" s="6">
-        <v>515</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.3">
@@ -5061,67 +5061,67 @@
       </c>
       <c r="D11" s="3">
         <f t="shared" si="0"/>
-        <v>692.15</v>
-      </c>
-      <c r="E11" s="6">
-        <v>703</v>
-      </c>
-      <c r="F11" s="6">
-        <v>688</v>
-      </c>
-      <c r="G11" s="6">
-        <v>703</v>
-      </c>
-      <c r="H11" s="6">
+        <v>689.4</v>
+      </c>
+      <c r="E11" s="19">
+        <v>685</v>
+      </c>
+      <c r="F11" s="19">
         <v>686</v>
       </c>
-      <c r="I11" s="6">
-        <v>688</v>
+      <c r="G11" s="19">
+        <v>686</v>
+      </c>
+      <c r="H11" s="19">
+        <v>687</v>
+      </c>
+      <c r="I11" s="19">
+        <v>687</v>
       </c>
       <c r="J11" s="6">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="K11" s="6">
-        <v>704</v>
+        <v>687</v>
       </c>
       <c r="L11" s="6">
-        <v>703</v>
+        <v>687</v>
       </c>
       <c r="M11" s="6">
         <v>688</v>
       </c>
       <c r="N11" s="6">
+        <v>688</v>
+      </c>
+      <c r="O11" s="6">
+        <v>688</v>
+      </c>
+      <c r="P11" s="6">
+        <v>688</v>
+      </c>
+      <c r="Q11" s="6">
         <v>689</v>
-      </c>
-      <c r="O11" s="6">
-        <v>704</v>
-      </c>
-      <c r="P11" s="6">
-        <v>687</v>
-      </c>
-      <c r="Q11" s="6">
-        <v>687</v>
       </c>
       <c r="R11" s="6">
         <v>689</v>
       </c>
       <c r="S11" s="6">
-        <v>687</v>
-      </c>
-      <c r="T11" s="6">
-        <v>687</v>
-      </c>
-      <c r="U11" s="6">
-        <v>687</v>
-      </c>
-      <c r="V11" s="6">
-        <v>686</v>
-      </c>
-      <c r="W11" s="5">
+        <v>703</v>
+      </c>
+      <c r="T11" s="19">
+        <v>703</v>
+      </c>
+      <c r="U11" s="19">
+        <v>703</v>
+      </c>
+      <c r="V11" s="19">
         <v>704</v>
       </c>
-      <c r="X11" s="6">
-        <v>688</v>
+      <c r="W11" s="22">
+        <v>704</v>
+      </c>
+      <c r="X11" s="19">
+        <v>704</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">
@@ -5133,67 +5133,67 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>1293.25</v>
-      </c>
-      <c r="E12" s="6">
-        <v>1306</v>
-      </c>
-      <c r="F12" s="6">
+        <v>1290.7</v>
+      </c>
+      <c r="E12" s="19">
+        <v>1285</v>
+      </c>
+      <c r="F12" s="19">
+        <v>1285</v>
+      </c>
+      <c r="G12" s="19">
+        <v>1286</v>
+      </c>
+      <c r="H12" s="19">
         <v>1287</v>
       </c>
-      <c r="G12" s="6">
-        <v>1306</v>
-      </c>
-      <c r="H12" s="6">
-        <v>1285</v>
-      </c>
-      <c r="I12" s="6">
-        <v>1290</v>
+      <c r="I12" s="19">
+        <v>1287</v>
       </c>
       <c r="J12" s="6">
         <v>1288</v>
       </c>
       <c r="K12" s="6">
+        <v>1288</v>
+      </c>
+      <c r="L12" s="6">
+        <v>1288</v>
+      </c>
+      <c r="M12" s="6">
+        <v>1289</v>
+      </c>
+      <c r="N12" s="6">
+        <v>1290</v>
+      </c>
+      <c r="O12" s="6">
+        <v>1290</v>
+      </c>
+      <c r="P12" s="6">
+        <v>1290</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>1290</v>
+      </c>
+      <c r="R12" s="6">
+        <v>1291</v>
+      </c>
+      <c r="S12" s="6">
+        <v>1303</v>
+      </c>
+      <c r="T12" s="19">
+        <v>1304</v>
+      </c>
+      <c r="U12" s="19">
         <v>1306</v>
       </c>
-      <c r="L12" s="6">
+      <c r="V12" s="19">
         <v>1306</v>
       </c>
-      <c r="M12" s="6">
-        <v>1290</v>
-      </c>
-      <c r="N12" s="6">
-        <v>1291</v>
-      </c>
-      <c r="O12" s="6">
-        <v>1303</v>
-      </c>
-      <c r="P12" s="6">
-        <v>1287</v>
-      </c>
-      <c r="Q12" s="6">
-        <v>1288</v>
-      </c>
-      <c r="R12" s="6">
-        <v>1289</v>
-      </c>
-      <c r="S12" s="6">
-        <v>1290</v>
-      </c>
-      <c r="T12" s="6">
-        <v>1285</v>
-      </c>
-      <c r="U12" s="6">
-        <v>1288</v>
-      </c>
-      <c r="V12" s="6">
-        <v>1286</v>
-      </c>
-      <c r="W12" s="5">
-        <v>1304</v>
-      </c>
-      <c r="X12" s="6">
-        <v>1290</v>
+      <c r="W12" s="22">
+        <v>1306</v>
+      </c>
+      <c r="X12" s="19">
+        <v>1306</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
@@ -5205,67 +5205,67 @@
       </c>
       <c r="D13" s="9">
         <f t="shared" si="0"/>
-        <v>522.75</v>
-      </c>
-      <c r="E13" s="10">
-        <v>533</v>
-      </c>
-      <c r="F13" s="10">
+        <v>523.5</v>
+      </c>
+      <c r="E13" s="26">
+        <v>510</v>
+      </c>
+      <c r="F13" s="26">
+        <v>510</v>
+      </c>
+      <c r="G13" s="26">
+        <v>510</v>
+      </c>
+      <c r="H13" s="26">
+        <v>511</v>
+      </c>
+      <c r="I13" s="26">
+        <v>514</v>
+      </c>
+      <c r="J13" s="10">
+        <v>514</v>
+      </c>
+      <c r="K13" s="10">
+        <v>515</v>
+      </c>
+      <c r="L13" s="10">
+        <v>516</v>
+      </c>
+      <c r="M13" s="10">
+        <v>517</v>
+      </c>
+      <c r="N13" s="10">
+        <v>517</v>
+      </c>
+      <c r="O13" s="10">
+        <v>530</v>
+      </c>
+      <c r="P13" s="10">
+        <v>531</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>531</v>
+      </c>
+      <c r="R13" s="10">
         <v>532</v>
-      </c>
-      <c r="G13" s="10">
-        <v>530</v>
-      </c>
-      <c r="H13" s="10">
-        <v>533</v>
-      </c>
-      <c r="I13" s="10">
-        <v>533</v>
-      </c>
-      <c r="J13" s="10">
-        <v>531</v>
-      </c>
-      <c r="K13" s="10">
-        <v>517</v>
-      </c>
-      <c r="L13" s="10">
-        <v>510</v>
-      </c>
-      <c r="M13" s="10">
-        <v>514</v>
-      </c>
-      <c r="N13" s="10">
-        <v>531</v>
-      </c>
-      <c r="O13" s="10">
-        <v>511</v>
-      </c>
-      <c r="P13" s="10">
-        <v>510</v>
-      </c>
-      <c r="Q13" s="10">
-        <v>517</v>
-      </c>
-      <c r="R13" s="10">
-        <v>516</v>
       </c>
       <c r="S13" s="10">
         <v>532</v>
       </c>
-      <c r="T13" s="10">
-        <v>514</v>
-      </c>
-      <c r="U13" s="10">
+      <c r="T13" s="26">
         <v>532</v>
       </c>
-      <c r="V13" s="10">
+      <c r="U13" s="26">
+        <v>533</v>
+      </c>
+      <c r="V13" s="26">
+        <v>533</v>
+      </c>
+      <c r="W13" s="27">
+        <v>533</v>
+      </c>
+      <c r="X13" s="26">
         <v>534</v>
-      </c>
-      <c r="W13" s="8">
-        <v>515</v>
-      </c>
-      <c r="X13" s="10">
-        <v>510</v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
@@ -5277,67 +5277,67 @@
       </c>
       <c r="D14" s="9">
         <f t="shared" si="0"/>
-        <v>697.65</v>
-      </c>
-      <c r="E14" s="10">
-        <v>705</v>
-      </c>
-      <c r="F14" s="10">
-        <v>703</v>
-      </c>
-      <c r="G14" s="10">
-        <v>706</v>
-      </c>
-      <c r="H14" s="10">
-        <v>703</v>
-      </c>
-      <c r="I14" s="10">
-        <v>705</v>
+        <v>699.4</v>
+      </c>
+      <c r="E14" s="26">
+        <v>685</v>
+      </c>
+      <c r="F14" s="26">
+        <v>686</v>
+      </c>
+      <c r="G14" s="26">
+        <v>686</v>
+      </c>
+      <c r="H14" s="26">
+        <v>686</v>
+      </c>
+      <c r="I14" s="26">
+        <v>687</v>
       </c>
       <c r="J14" s="10">
-        <v>707</v>
+        <v>691</v>
       </c>
       <c r="K14" s="10">
         <v>691</v>
       </c>
       <c r="L14" s="10">
-        <v>685</v>
+        <v>691</v>
       </c>
       <c r="M14" s="10">
-        <v>686</v>
+        <v>701</v>
       </c>
       <c r="N14" s="10">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="O14" s="10">
         <v>703</v>
       </c>
       <c r="P14" s="10">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="Q14" s="10">
-        <v>691</v>
+        <v>703</v>
       </c>
       <c r="R14" s="10">
-        <v>691</v>
+        <v>704</v>
       </c>
       <c r="S14" s="10">
         <v>705</v>
       </c>
-      <c r="T14" s="10">
-        <v>686</v>
-      </c>
-      <c r="U14" s="10">
+      <c r="T14" s="26">
+        <v>705</v>
+      </c>
+      <c r="U14" s="26">
+        <v>705</v>
+      </c>
+      <c r="V14" s="26">
         <v>706</v>
       </c>
-      <c r="V14" s="10">
-        <v>704</v>
-      </c>
-      <c r="W14" s="8">
-        <v>687</v>
-      </c>
-      <c r="X14" s="10">
-        <v>686</v>
+      <c r="W14" s="27">
+        <v>706</v>
+      </c>
+      <c r="X14" s="26">
+        <v>707</v>
       </c>
     </row>
     <row r="15" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5349,67 +5349,67 @@
       </c>
       <c r="D15" s="9">
         <f t="shared" si="0"/>
-        <v>1298.2</v>
-      </c>
-      <c r="E15" s="10">
-        <v>1308</v>
-      </c>
-      <c r="F15" s="10">
+        <v>1299.5999999999999</v>
+      </c>
+      <c r="E15" s="26">
+        <v>1286</v>
+      </c>
+      <c r="F15" s="26">
+        <v>1286</v>
+      </c>
+      <c r="G15" s="26">
+        <v>1286</v>
+      </c>
+      <c r="H15" s="26">
+        <v>1287</v>
+      </c>
+      <c r="I15" s="26">
+        <v>1288</v>
+      </c>
+      <c r="J15" s="10">
+        <v>1289</v>
+      </c>
+      <c r="K15" s="10">
+        <v>1289</v>
+      </c>
+      <c r="L15" s="10">
+        <v>1289</v>
+      </c>
+      <c r="M15" s="10">
         <v>1302</v>
       </c>
-      <c r="G15" s="10">
-        <v>1305</v>
-      </c>
-      <c r="H15" s="10">
-        <v>1306</v>
-      </c>
-      <c r="I15" s="10">
-        <v>1305</v>
-      </c>
-      <c r="J15" s="10">
-        <v>1306</v>
-      </c>
-      <c r="K15" s="10">
-        <v>1287</v>
-      </c>
-      <c r="L15" s="10">
-        <v>1286</v>
-      </c>
-      <c r="M15" s="10">
-        <v>1289</v>
-      </c>
       <c r="N15" s="10">
-        <v>1307</v>
+        <v>1303</v>
       </c>
       <c r="O15" s="10">
         <v>1304</v>
       </c>
       <c r="P15" s="10">
+        <v>1304</v>
+      </c>
+      <c r="Q15" s="10">
+        <v>1305</v>
+      </c>
+      <c r="R15" s="10">
+        <v>1305</v>
+      </c>
+      <c r="S15" s="10">
+        <v>1306</v>
+      </c>
+      <c r="T15" s="26">
+        <v>1306</v>
+      </c>
+      <c r="U15" s="26">
         <v>1307</v>
       </c>
-      <c r="Q15" s="10">
-        <v>1289</v>
-      </c>
-      <c r="R15" s="10">
-        <v>1286</v>
-      </c>
-      <c r="S15" s="10">
+      <c r="V15" s="26">
         <v>1307</v>
       </c>
-      <c r="T15" s="10">
-        <v>1288</v>
-      </c>
-      <c r="U15" s="10">
-        <v>1303</v>
-      </c>
-      <c r="V15" s="10">
-        <v>1304</v>
-      </c>
-      <c r="W15" s="8">
-        <v>1289</v>
-      </c>
-      <c r="X15" s="10">
-        <v>1286</v>
+      <c r="W15" s="27">
+        <v>1307</v>
+      </c>
+      <c r="X15" s="26">
+        <v>1308</v>
       </c>
     </row>
     <row r="17" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5427,19 +5427,19 @@
       <c r="D18" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="23">
         <v>1</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="23">
         <v>2</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="23">
         <v>3</v>
       </c>
-      <c r="H18" s="17">
+      <c r="H18" s="23">
         <v>4</v>
       </c>
-      <c r="I18" s="17">
+      <c r="I18" s="23">
         <v>5</v>
       </c>
       <c r="J18" s="17">
@@ -5472,19 +5472,19 @@
       <c r="S18" s="17">
         <v>15</v>
       </c>
-      <c r="T18" s="17">
+      <c r="T18" s="23">
         <v>16</v>
       </c>
-      <c r="U18" s="17">
+      <c r="U18" s="23">
         <v>17</v>
       </c>
-      <c r="V18" s="17">
+      <c r="V18" s="23">
         <v>18</v>
       </c>
-      <c r="W18" s="16">
+      <c r="W18" s="24">
         <v>19</v>
       </c>
-      <c r="X18" s="17">
+      <c r="X18" s="23">
         <v>20</v>
       </c>
     </row>
@@ -5496,22 +5496,22 @@
         <v>1</v>
       </c>
       <c r="D19" s="3">
-        <f>AVERAGE(E19:AC19)</f>
-        <v>261</v>
-      </c>
-      <c r="E19" s="3">
-        <v>261</v>
-      </c>
-      <c r="F19" s="3">
-        <v>261</v>
-      </c>
-      <c r="G19" s="3">
-        <v>261</v>
-      </c>
-      <c r="H19" s="3">
-        <v>261</v>
-      </c>
-      <c r="I19" s="3">
+        <f>AVERAGE(J19:S19)</f>
+        <v>261</v>
+      </c>
+      <c r="E19" s="18">
+        <v>261</v>
+      </c>
+      <c r="F19" s="18">
+        <v>261</v>
+      </c>
+      <c r="G19" s="18">
+        <v>261</v>
+      </c>
+      <c r="H19" s="18">
+        <v>261</v>
+      </c>
+      <c r="I19" s="18">
         <v>261</v>
       </c>
       <c r="J19" s="3">
@@ -5544,19 +5544,19 @@
       <c r="S19" s="3">
         <v>261</v>
       </c>
-      <c r="T19" s="3">
-        <v>261</v>
-      </c>
-      <c r="U19" s="3">
-        <v>261</v>
-      </c>
-      <c r="V19" s="3">
-        <v>261</v>
-      </c>
-      <c r="W19" s="3">
-        <v>261</v>
-      </c>
-      <c r="X19" s="3">
+      <c r="T19" s="18">
+        <v>261</v>
+      </c>
+      <c r="U19" s="18">
+        <v>261</v>
+      </c>
+      <c r="V19" s="18">
+        <v>261</v>
+      </c>
+      <c r="W19" s="18">
+        <v>261</v>
+      </c>
+      <c r="X19" s="18">
         <v>261</v>
       </c>
     </row>
@@ -5568,22 +5568,22 @@
         <v>2</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" ref="D20:D21" si="1">AVERAGE(E20:AC20)</f>
-        <v>476</v>
-      </c>
-      <c r="E20" s="6">
-        <v>476</v>
-      </c>
-      <c r="F20" s="6">
-        <v>476</v>
-      </c>
-      <c r="G20" s="6">
-        <v>476</v>
-      </c>
-      <c r="H20" s="6">
-        <v>476</v>
-      </c>
-      <c r="I20" s="6">
+        <f t="shared" ref="D20:D30" si="1">AVERAGE(J20:S20)</f>
+        <v>476</v>
+      </c>
+      <c r="E20" s="19">
+        <v>476</v>
+      </c>
+      <c r="F20" s="19">
+        <v>476</v>
+      </c>
+      <c r="G20" s="19">
+        <v>476</v>
+      </c>
+      <c r="H20" s="19">
+        <v>476</v>
+      </c>
+      <c r="I20" s="19">
         <v>476</v>
       </c>
       <c r="J20" s="6">
@@ -5616,19 +5616,19 @@
       <c r="S20" s="6">
         <v>476</v>
       </c>
-      <c r="T20" s="6">
-        <v>476</v>
-      </c>
-      <c r="U20" s="6">
-        <v>476</v>
-      </c>
-      <c r="V20" s="6">
-        <v>476</v>
-      </c>
-      <c r="W20" s="6">
-        <v>476</v>
-      </c>
-      <c r="X20" s="6">
+      <c r="T20" s="19">
+        <v>476</v>
+      </c>
+      <c r="U20" s="19">
+        <v>476</v>
+      </c>
+      <c r="V20" s="19">
+        <v>476</v>
+      </c>
+      <c r="W20" s="19">
+        <v>476</v>
+      </c>
+      <c r="X20" s="19">
         <v>476</v>
       </c>
     </row>
@@ -5643,19 +5643,19 @@
         <f t="shared" si="1"/>
         <v>1330</v>
       </c>
-      <c r="E21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="F21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="G21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="H21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="I21" s="6">
+      <c r="E21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="F21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="G21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="H21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="I21" s="19">
         <v>1330</v>
       </c>
       <c r="J21" s="6">
@@ -5688,19 +5688,19 @@
       <c r="S21" s="6">
         <v>1330</v>
       </c>
-      <c r="T21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="U21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="V21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="W21" s="6">
-        <v>1330</v>
-      </c>
-      <c r="X21" s="6">
+      <c r="T21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="U21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="V21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="W21" s="19">
+        <v>1330</v>
+      </c>
+      <c r="X21" s="19">
         <v>1330</v>
       </c>
     </row>
@@ -5712,22 +5712,22 @@
         <v>1</v>
       </c>
       <c r="D22" s="9">
-        <f t="shared" ref="D22:D30" si="2">AVERAGE(E22:AC22)</f>
-        <v>261</v>
-      </c>
-      <c r="E22" s="9">
-        <v>261</v>
-      </c>
-      <c r="F22" s="9">
-        <v>261</v>
-      </c>
-      <c r="G22" s="9">
-        <v>261</v>
-      </c>
-      <c r="H22" s="9">
-        <v>261</v>
-      </c>
-      <c r="I22" s="9">
+        <f t="shared" si="1"/>
+        <v>261</v>
+      </c>
+      <c r="E22" s="25">
+        <v>261</v>
+      </c>
+      <c r="F22" s="25">
+        <v>261</v>
+      </c>
+      <c r="G22" s="25">
+        <v>261</v>
+      </c>
+      <c r="H22" s="25">
+        <v>261</v>
+      </c>
+      <c r="I22" s="25">
         <v>261</v>
       </c>
       <c r="J22" s="9">
@@ -5760,19 +5760,19 @@
       <c r="S22" s="9">
         <v>261</v>
       </c>
-      <c r="T22" s="9">
-        <v>261</v>
-      </c>
-      <c r="U22" s="9">
-        <v>261</v>
-      </c>
-      <c r="V22" s="9">
-        <v>261</v>
-      </c>
-      <c r="W22" s="9">
-        <v>261</v>
-      </c>
-      <c r="X22" s="9">
+      <c r="T22" s="25">
+        <v>261</v>
+      </c>
+      <c r="U22" s="25">
+        <v>261</v>
+      </c>
+      <c r="V22" s="25">
+        <v>261</v>
+      </c>
+      <c r="W22" s="25">
+        <v>261</v>
+      </c>
+      <c r="X22" s="25">
         <v>261</v>
       </c>
     </row>
@@ -5784,22 +5784,22 @@
         <v>2</v>
       </c>
       <c r="D23" s="9">
-        <f t="shared" si="2"/>
-        <v>476</v>
-      </c>
-      <c r="E23" s="10">
-        <v>476</v>
-      </c>
-      <c r="F23" s="10">
-        <v>476</v>
-      </c>
-      <c r="G23" s="10">
-        <v>476</v>
-      </c>
-      <c r="H23" s="10">
-        <v>476</v>
-      </c>
-      <c r="I23" s="10">
+        <f t="shared" si="1"/>
+        <v>476</v>
+      </c>
+      <c r="E23" s="26">
+        <v>476</v>
+      </c>
+      <c r="F23" s="26">
+        <v>476</v>
+      </c>
+      <c r="G23" s="26">
+        <v>476</v>
+      </c>
+      <c r="H23" s="26">
+        <v>476</v>
+      </c>
+      <c r="I23" s="26">
         <v>476</v>
       </c>
       <c r="J23" s="10">
@@ -5832,19 +5832,19 @@
       <c r="S23" s="10">
         <v>476</v>
       </c>
-      <c r="T23" s="10">
-        <v>476</v>
-      </c>
-      <c r="U23" s="10">
-        <v>476</v>
-      </c>
-      <c r="V23" s="10">
-        <v>476</v>
-      </c>
-      <c r="W23" s="10">
-        <v>476</v>
-      </c>
-      <c r="X23" s="10">
+      <c r="T23" s="26">
+        <v>476</v>
+      </c>
+      <c r="U23" s="26">
+        <v>476</v>
+      </c>
+      <c r="V23" s="26">
+        <v>476</v>
+      </c>
+      <c r="W23" s="26">
+        <v>476</v>
+      </c>
+      <c r="X23" s="26">
         <v>476</v>
       </c>
     </row>
@@ -5856,22 +5856,22 @@
         <v>3</v>
       </c>
       <c r="D24" s="9">
-        <f t="shared" si="2"/>
-        <v>1330</v>
-      </c>
-      <c r="E24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="F24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="G24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="H24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="I24" s="10">
+        <f t="shared" si="1"/>
+        <v>1330</v>
+      </c>
+      <c r="E24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="F24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="G24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="H24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="I24" s="26">
         <v>1330</v>
       </c>
       <c r="J24" s="10">
@@ -5904,19 +5904,19 @@
       <c r="S24" s="10">
         <v>1330</v>
       </c>
-      <c r="T24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="U24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="V24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="W24" s="10">
-        <v>1330</v>
-      </c>
-      <c r="X24" s="10">
+      <c r="T24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="U24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="V24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="W24" s="26">
+        <v>1330</v>
+      </c>
+      <c r="X24" s="26">
         <v>1330</v>
       </c>
     </row>
@@ -5928,22 +5928,22 @@
         <v>1</v>
       </c>
       <c r="D25" s="3">
-        <f t="shared" si="2"/>
-        <v>261</v>
-      </c>
-      <c r="E25" s="3">
-        <v>261</v>
-      </c>
-      <c r="F25" s="3">
-        <v>261</v>
-      </c>
-      <c r="G25" s="3">
-        <v>261</v>
-      </c>
-      <c r="H25" s="3">
-        <v>261</v>
-      </c>
-      <c r="I25" s="3">
+        <f t="shared" si="1"/>
+        <v>261</v>
+      </c>
+      <c r="E25" s="18">
+        <v>261</v>
+      </c>
+      <c r="F25" s="18">
+        <v>261</v>
+      </c>
+      <c r="G25" s="18">
+        <v>261</v>
+      </c>
+      <c r="H25" s="18">
+        <v>261</v>
+      </c>
+      <c r="I25" s="18">
         <v>261</v>
       </c>
       <c r="J25" s="3">
@@ -5976,19 +5976,19 @@
       <c r="S25" s="3">
         <v>261</v>
       </c>
-      <c r="T25" s="3">
-        <v>261</v>
-      </c>
-      <c r="U25" s="3">
-        <v>261</v>
-      </c>
-      <c r="V25" s="3">
-        <v>261</v>
-      </c>
-      <c r="W25" s="3">
-        <v>261</v>
-      </c>
-      <c r="X25" s="3">
+      <c r="T25" s="18">
+        <v>261</v>
+      </c>
+      <c r="U25" s="18">
+        <v>261</v>
+      </c>
+      <c r="V25" s="18">
+        <v>261</v>
+      </c>
+      <c r="W25" s="18">
+        <v>261</v>
+      </c>
+      <c r="X25" s="18">
         <v>261</v>
       </c>
     </row>
@@ -6000,22 +6000,22 @@
         <v>2</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" si="2"/>
-        <v>476</v>
-      </c>
-      <c r="E26" s="6">
-        <v>476</v>
-      </c>
-      <c r="F26" s="6">
-        <v>476</v>
-      </c>
-      <c r="G26" s="6">
-        <v>476</v>
-      </c>
-      <c r="H26" s="6">
-        <v>476</v>
-      </c>
-      <c r="I26" s="6">
+        <f t="shared" si="1"/>
+        <v>476</v>
+      </c>
+      <c r="E26" s="19">
+        <v>476</v>
+      </c>
+      <c r="F26" s="19">
+        <v>476</v>
+      </c>
+      <c r="G26" s="19">
+        <v>476</v>
+      </c>
+      <c r="H26" s="19">
+        <v>476</v>
+      </c>
+      <c r="I26" s="19">
         <v>476</v>
       </c>
       <c r="J26" s="6">
@@ -6048,19 +6048,19 @@
       <c r="S26" s="6">
         <v>476</v>
       </c>
-      <c r="T26" s="6">
-        <v>476</v>
-      </c>
-      <c r="U26" s="6">
-        <v>476</v>
-      </c>
-      <c r="V26" s="6">
-        <v>476</v>
-      </c>
-      <c r="W26" s="6">
-        <v>476</v>
-      </c>
-      <c r="X26" s="6">
+      <c r="T26" s="19">
+        <v>476</v>
+      </c>
+      <c r="U26" s="19">
+        <v>476</v>
+      </c>
+      <c r="V26" s="19">
+        <v>476</v>
+      </c>
+      <c r="W26" s="19">
+        <v>476</v>
+      </c>
+      <c r="X26" s="19">
         <v>476</v>
       </c>
     </row>
@@ -6072,22 +6072,22 @@
         <v>3</v>
       </c>
       <c r="D27" s="3">
-        <f t="shared" si="2"/>
-        <v>1330</v>
-      </c>
-      <c r="E27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="F27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="G27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="H27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="I27" s="6">
+        <f t="shared" si="1"/>
+        <v>1330</v>
+      </c>
+      <c r="E27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="F27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="G27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="H27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="I27" s="19">
         <v>1330</v>
       </c>
       <c r="J27" s="6">
@@ -6120,19 +6120,19 @@
       <c r="S27" s="6">
         <v>1330</v>
       </c>
-      <c r="T27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="U27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="V27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="W27" s="6">
-        <v>1330</v>
-      </c>
-      <c r="X27" s="6">
+      <c r="T27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="U27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="V27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="W27" s="19">
+        <v>1330</v>
+      </c>
+      <c r="X27" s="19">
         <v>1330</v>
       </c>
     </row>
@@ -6144,22 +6144,22 @@
         <v>1</v>
       </c>
       <c r="D28" s="9">
-        <f t="shared" si="2"/>
-        <v>261</v>
-      </c>
-      <c r="E28" s="9">
-        <v>261</v>
-      </c>
-      <c r="F28" s="9">
-        <v>261</v>
-      </c>
-      <c r="G28" s="9">
-        <v>261</v>
-      </c>
-      <c r="H28" s="9">
-        <v>261</v>
-      </c>
-      <c r="I28" s="9">
+        <f t="shared" si="1"/>
+        <v>261</v>
+      </c>
+      <c r="E28" s="25">
+        <v>261</v>
+      </c>
+      <c r="F28" s="25">
+        <v>261</v>
+      </c>
+      <c r="G28" s="25">
+        <v>261</v>
+      </c>
+      <c r="H28" s="25">
+        <v>261</v>
+      </c>
+      <c r="I28" s="25">
         <v>261</v>
       </c>
       <c r="J28" s="9">
@@ -6192,19 +6192,19 @@
       <c r="S28" s="9">
         <v>261</v>
       </c>
-      <c r="T28" s="9">
-        <v>261</v>
-      </c>
-      <c r="U28" s="9">
-        <v>261</v>
-      </c>
-      <c r="V28" s="9">
-        <v>261</v>
-      </c>
-      <c r="W28" s="9">
-        <v>261</v>
-      </c>
-      <c r="X28" s="9">
+      <c r="T28" s="25">
+        <v>261</v>
+      </c>
+      <c r="U28" s="25">
+        <v>261</v>
+      </c>
+      <c r="V28" s="25">
+        <v>261</v>
+      </c>
+      <c r="W28" s="25">
+        <v>261</v>
+      </c>
+      <c r="X28" s="25">
         <v>261</v>
       </c>
     </row>
@@ -6216,22 +6216,22 @@
         <v>2</v>
       </c>
       <c r="D29" s="9">
-        <f t="shared" si="2"/>
-        <v>476</v>
-      </c>
-      <c r="E29" s="10">
-        <v>476</v>
-      </c>
-      <c r="F29" s="10">
-        <v>476</v>
-      </c>
-      <c r="G29" s="10">
-        <v>476</v>
-      </c>
-      <c r="H29" s="10">
-        <v>476</v>
-      </c>
-      <c r="I29" s="10">
+        <f t="shared" si="1"/>
+        <v>476</v>
+      </c>
+      <c r="E29" s="26">
+        <v>476</v>
+      </c>
+      <c r="F29" s="26">
+        <v>476</v>
+      </c>
+      <c r="G29" s="26">
+        <v>476</v>
+      </c>
+      <c r="H29" s="26">
+        <v>476</v>
+      </c>
+      <c r="I29" s="26">
         <v>476</v>
       </c>
       <c r="J29" s="10">
@@ -6264,19 +6264,19 @@
       <c r="S29" s="10">
         <v>476</v>
       </c>
-      <c r="T29" s="10">
-        <v>476</v>
-      </c>
-      <c r="U29" s="10">
-        <v>476</v>
-      </c>
-      <c r="V29" s="10">
-        <v>476</v>
-      </c>
-      <c r="W29" s="10">
-        <v>476</v>
-      </c>
-      <c r="X29" s="10">
+      <c r="T29" s="26">
+        <v>476</v>
+      </c>
+      <c r="U29" s="26">
+        <v>476</v>
+      </c>
+      <c r="V29" s="26">
+        <v>476</v>
+      </c>
+      <c r="W29" s="26">
+        <v>476</v>
+      </c>
+      <c r="X29" s="26">
         <v>476</v>
       </c>
     </row>
@@ -6288,22 +6288,22 @@
         <v>3</v>
       </c>
       <c r="D30" s="9">
-        <f t="shared" si="2"/>
-        <v>1330</v>
-      </c>
-      <c r="E30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="F30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="G30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="H30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="I30" s="10">
+        <f t="shared" si="1"/>
+        <v>1330</v>
+      </c>
+      <c r="E30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="F30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="G30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="H30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="I30" s="26">
         <v>1330</v>
       </c>
       <c r="J30" s="10">
@@ -6336,25 +6336,25 @@
       <c r="S30" s="10">
         <v>1330</v>
       </c>
-      <c r="T30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="U30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="V30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="W30" s="10">
-        <v>1330</v>
-      </c>
-      <c r="X30" s="10">
+      <c r="T30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="U30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="V30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="W30" s="26">
+        <v>1330</v>
+      </c>
+      <c r="X30" s="26">
         <v>1330</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E4:X4">
-    <sortCondition ref="X4"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="E15:X15">
+    <sortCondition ref="E15:X15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>